<commit_message>
Tab Insurance Partial Setting
</commit_message>
<xml_diff>
--- a/Excel/2.1 DataFile_NAP_CF4W.xlsx
+++ b/Excel/2.1 DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17385" windowHeight="6630" tabRatio="769" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17385" windowHeight="6630" tabRatio="769" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -14568,7 +14568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0" shapeId="0">
+    <comment ref="B88" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -14957,7 +14957,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4885" uniqueCount="3519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4886" uniqueCount="3529">
   <si>
     <t>Count</t>
   </si>
@@ -25514,13 +25514,43 @@
     <t>2;3;1</t>
   </si>
   <si>
-    <t>3805000</t>
-  </si>
-  <si>
     <t>0002APP20211203568</t>
   </si>
   <si>
     <t>MO Notes</t>
+  </si>
+  <si>
+    <t>Capitalize if GS_Value Partial</t>
+  </si>
+  <si>
+    <t>Full Capitalize Amount</t>
+  </si>
+  <si>
+    <t>Capitalize Amount</t>
+  </si>
+  <si>
+    <t>Button Save Tidak Berfungsi</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>CountofFamily</t>
+  </si>
+  <si>
+    <t>CountofGuarantorPersonal</t>
+  </si>
+  <si>
+    <t>CountofGuarantorCompany</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Multifinance;multifinance;multifinance</t>
+  </si>
+  <si>
+    <t>17503000</t>
   </si>
 </sst>
 </file>
@@ -26029,7 +26059,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -26202,6 +26232,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -26288,7 +26319,194 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="154">
+  <dxfs count="155">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -26950,186 +27168,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -27719,8 +27757,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="QueryJobProfessionEmployee" displayName="QueryJobProfessionEmployee" ref="A1:B43" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B43"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION EMP" queryTableFieldId="1" dataDxfId="153"/>
-    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="152"/>
+    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION EMP" queryTableFieldId="1" dataDxfId="59"/>
+    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27730,7 +27768,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="QueryGuarantorRelationshipPersonal" displayName="QueryGuarantorRelationshipPersonal" ref="AB1:AB14" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AB1:AB14"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="GUARANTOR_RELATIONSHIP_PERSONAL" queryTableFieldId="1" dataDxfId="139"/>
+    <tableColumn id="1" uniqueName="1" name="GUARANTOR_RELATIONSHIP_PERSONAL" queryTableFieldId="1" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27740,7 +27778,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="QueryGender" displayName="QueryGender" ref="AD1:AD3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AD1:AD3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="GENDER" queryTableFieldId="1" dataDxfId="138"/>
+    <tableColumn id="1" uniqueName="1" name="GENDER" queryTableFieldId="1" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27750,7 +27788,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="QueryCustomerModelPersonal" displayName="QueryCustomerModelPersonal" ref="AF1:AF5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AF1:AF5"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="CUSTOMER MODEL PERSONAL" queryTableFieldId="1" dataDxfId="137"/>
+    <tableColumn id="1" uniqueName="1" name="CUSTOMER MODEL PERSONAL" queryTableFieldId="1" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27760,7 +27798,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="QueryGuarantorRelationshipCompany" displayName="QueryGuarantorRelationshipCompany" ref="AH1:AH7" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AH1:AH7"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="GUARANTOR_RELATIONSHIP_COMPANY" queryTableFieldId="1" dataDxfId="136"/>
+    <tableColumn id="1" uniqueName="1" name="GUARANTOR_RELATIONSHIP_COMPANY" queryTableFieldId="1" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27770,7 +27808,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="QueryCustomerModelCompany" displayName="QueryCustomerModelCompany" ref="AJ1:AJ3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AJ1:AJ3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="CUSTOMER MODEL COMPANY" queryTableFieldId="1" dataDxfId="135"/>
+    <tableColumn id="1" uniqueName="1" name="CUSTOMER MODEL COMPANY" queryTableFieldId="1" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27780,7 +27818,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="QueryCompanyType" displayName="QueryCompanyType" ref="AL1:AL6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AL1:AL6"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="COMPANY TYPE" queryTableFieldId="1" dataDxfId="134"/>
+    <tableColumn id="1" uniqueName="1" name="COMPANY TYPE" queryTableFieldId="1" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27790,7 +27828,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="QueryLifeInscoBranchName" displayName="QueryLifeInscoBranchName" ref="AN1:AN30" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AN1:AN30"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="LIFE INSCO BRANCH NAME" queryTableFieldId="1" dataDxfId="133"/>
+    <tableColumn id="1" uniqueName="1" name="LIFE INSCO BRANCH NAME" queryTableFieldId="1" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27800,7 +27838,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="QueryPremiumPaymentMethod" displayName="QueryPremiumPaymentMethod" ref="AP1:AP4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AP1:AP4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Premium Payment Method" queryTableFieldId="1" dataDxfId="132"/>
+    <tableColumn id="1" uniqueName="1" name="Premium Payment Method" queryTableFieldId="1" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27810,8 +27848,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="QueryEconomicSectorSLIK" displayName="QueryEconomicSectorSLIK" ref="AR1:AS476" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AR1:AS476"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="ECONOMIC SECTOR NAME" queryTableFieldId="1" dataDxfId="131"/>
-    <tableColumn id="2" uniqueName="2" name="ECONOMIC SECTOR CODE" queryTableFieldId="2" dataDxfId="130"/>
+    <tableColumn id="1" uniqueName="1" name="ECONOMIC SECTOR NAME" queryTableFieldId="1" dataDxfId="37"/>
+    <tableColumn id="2" uniqueName="2" name="ECONOMIC SECTOR CODE" queryTableFieldId="2" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27821,8 +27859,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Query_Ref_Master_App_Data" displayName="Query_Ref_Master_App_Data" ref="AU1:AV5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AU1:AV5"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="REF MASTER APPDATA DESCRIPTION" queryTableFieldId="1" dataDxfId="129"/>
-    <tableColumn id="2" uniqueName="2" name="REF MASTER APPDATA CODE" queryTableFieldId="2" dataDxfId="128"/>
+    <tableColumn id="1" uniqueName="1" name="REF MASTER APPDATA DESCRIPTION" queryTableFieldId="1" dataDxfId="35"/>
+    <tableColumn id="2" uniqueName="2" name="REF MASTER APPDATA CODE" queryTableFieldId="2" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27832,8 +27870,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="QueryCountry" displayName="QueryCountry" ref="E1:F242" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="E1:F242"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="COUNTRY NAME" queryTableFieldId="1" dataDxfId="151"/>
-    <tableColumn id="2" uniqueName="2" name="COUNTRY CODE" queryTableFieldId="2" dataDxfId="150"/>
+    <tableColumn id="1" uniqueName="1" name="COUNTRY NAME" queryTableFieldId="1" dataDxfId="57"/>
+    <tableColumn id="2" uniqueName="2" name="COUNTRY CODE" queryTableFieldId="2" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27843,7 +27881,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Query_Application_Source" displayName="Query_Application_Source" ref="AX1:AX16" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AX1:AX16"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="APPLICATION SOURCE" queryTableFieldId="1" dataDxfId="127"/>
+    <tableColumn id="1" uniqueName="1" name="APPLICATION SOURCE" queryTableFieldId="1" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27853,7 +27891,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Query_First_Installment_Type" displayName="Query_First_Installment_Type" ref="AZ1:AZ3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="AZ1:AZ3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="FIRST INSTALLMENT TYPE" queryTableFieldId="1" dataDxfId="126"/>
+    <tableColumn id="1" uniqueName="1" name="FIRST INSTALLMENT TYPE" queryTableFieldId="1" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27863,7 +27901,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Query_Payment_Frequency" displayName="Query_Payment_Frequency" ref="BB1:BB17" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BB1:BB17"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="PAYMENT FREQUENCY" queryTableFieldId="1" dataDxfId="125"/>
+    <tableColumn id="1" uniqueName="1" name="PAYMENT FREQUENCY" queryTableFieldId="1" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27873,7 +27911,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Query_DP_Source_Payment_Type" displayName="Query_DP_Source_Payment_Type" ref="BD1:BD10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BD1:BD10"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="DP SOURCE PAYMENT TYPE" queryTableFieldId="1" dataDxfId="124"/>
+    <tableColumn id="1" uniqueName="1" name="DP SOURCE PAYMENT TYPE" queryTableFieldId="1" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27883,7 +27921,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Query_Interest_Type" displayName="Query_Interest_Type" ref="BF1:BF3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BF1:BF3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Interest Type" queryTableFieldId="1" dataDxfId="123"/>
+    <tableColumn id="1" uniqueName="1" name="Interest Type" queryTableFieldId="1" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27893,7 +27931,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Query_Installment_Scheme" displayName="Query_Installment_Scheme" ref="BH1:BH8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BH1:BH8"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="INSTALLMENT SCHEME" queryTableFieldId="1" dataDxfId="122"/>
+    <tableColumn id="1" uniqueName="1" name="INSTALLMENT SCHEME" queryTableFieldId="1" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27903,7 +27941,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Query_Floating_Period" displayName="Query_Floating_Period" ref="BJ1:BJ17" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BJ1:BJ17"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="FLOATING PERIOD" queryTableFieldId="1" dataDxfId="121"/>
+    <tableColumn id="1" uniqueName="1" name="FLOATING PERIOD" queryTableFieldId="1" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27913,7 +27951,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Query_WOP" displayName="Query_WOP" ref="BL1:BL6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BL1:BL6"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="WOP" queryTableFieldId="1" dataDxfId="120"/>
+    <tableColumn id="1" uniqueName="1" name="WOP" queryTableFieldId="1" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27923,7 +27961,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Query_Customer_Notification" displayName="Query_Customer_Notification" ref="BN1:BN4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BN1:BN4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="CUSTOMER NOTIFICATION BY" queryTableFieldId="1" dataDxfId="119"/>
+    <tableColumn id="1" uniqueName="1" name="CUSTOMER NOTIFICATION BY" queryTableFieldId="1" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27933,7 +27971,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Query_Installment_Source_Payment_Type" displayName="Query_Installment_Source_Payment_Type" ref="BP1:BP10" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BP1:BP10"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="INSTALLMENT SOURCE PAYMENT TYPE" queryTableFieldId="1" dataDxfId="118"/>
+    <tableColumn id="1" uniqueName="1" name="INSTALLMENT SOURCE PAYMENT TYPE" queryTableFieldId="1" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27943,8 +27981,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="QueryJobPosition" displayName="QueryJobPosition" ref="I1:J30" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="I1:J30"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="JOB POSITION NAME" queryTableFieldId="1" dataDxfId="149"/>
-    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="148"/>
+    <tableColumn id="1" uniqueName="1" name="JOB POSITION NAME" queryTableFieldId="1" dataDxfId="55"/>
+    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27953,7 +27991,7 @@
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Query_Copy_Address_From_App_Data_Personal" displayName="Query_Copy_Address_From_App_Data_Personal" ref="BR3:BR11" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="descr" queryTableFieldId="1" dataDxfId="117"/>
+    <tableColumn id="1" uniqueName="1" name="descr" queryTableFieldId="1" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27963,7 +28001,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Query_Characteristic_Of_Credit" displayName="Query_Characteristic_Of_Credit" ref="BT1:BT3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BT1:BT3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="CHARACTERISTIC OF CREDIT" queryTableFieldId="1" dataDxfId="116"/>
+    <tableColumn id="1" uniqueName="1" name="CHARACTERISTIC OF CREDIT" queryTableFieldId="1" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27973,7 +28011,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Query_Way_Of_Restructure" displayName="Query_Way_Of_Restructure" ref="BV1:BV4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BV1:BV4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="WAY OF RESTRUCTURE" queryTableFieldId="1" dataDxfId="115"/>
+    <tableColumn id="1" uniqueName="1" name="WAY OF RESTRUCTURE" queryTableFieldId="1" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27982,7 +28020,7 @@
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Query_Copy_Address_From_Asset_Data_Personal" displayName="Query_Copy_Address_From_Asset_Data_Personal" ref="BX2:BX10" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="master_code" queryTableFieldId="1" dataDxfId="114"/>
+    <tableColumn id="1" uniqueName="1" name="master_code" queryTableFieldId="1" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27992,7 +28030,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Query_Insured_By" displayName="Query_Insured_By" ref="BZ1:BZ5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="BZ1:BZ5"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="INSURED BY" queryTableFieldId="1" dataDxfId="113"/>
+    <tableColumn id="1" uniqueName="1" name="INSURED BY" queryTableFieldId="1" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28002,7 +28040,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Query_Asset_Region" displayName="Query_Asset_Region" ref="CB1:CB5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CB1:CB5"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="ASSET REGION" queryTableFieldId="1" dataDxfId="112"/>
+    <tableColumn id="1" uniqueName="1" name="ASSET REGION" queryTableFieldId="1" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28012,7 +28050,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Query_Cover_Period" displayName="Query_Cover_Period" ref="CD1:CD5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CD1:CD5"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="COVER PERIOD" queryTableFieldId="1" dataDxfId="111"/>
+    <tableColumn id="1" uniqueName="1" name="COVER PERIOD" queryTableFieldId="1" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28022,7 +28060,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Query_Payment_Type" displayName="Query_Payment_Type" ref="CF1:CF3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CF1:CF3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="PAYMENT TYPE" queryTableFieldId="1" dataDxfId="110"/>
+    <tableColumn id="1" uniqueName="1" name="PAYMENT TYPE" queryTableFieldId="1" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28032,7 +28070,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Query_Asset_Insco_Branch_Name" displayName="Query_Asset_Insco_Branch_Name" ref="CH1:CH30" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CH1:CH30"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="INSCO BRANCH NAME" queryTableFieldId="1" dataDxfId="109"/>
+    <tableColumn id="1" uniqueName="1" name="INSCO BRANCH NAME" queryTableFieldId="1" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28042,7 +28080,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="Query_Insurance_Main_Coverage" displayName="Query_Insurance_Main_Coverage" ref="CJ1:CJ4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CJ1:CJ4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="INSURANCE MAIN COVERAGE" queryTableFieldId="1" dataDxfId="108"/>
+    <tableColumn id="1" uniqueName="1" name="INSURANCE MAIN COVERAGE" queryTableFieldId="1" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28052,8 +28090,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="QueryDepartmentAML" displayName="QueryDepartmentAML" ref="M1:N492" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="M1:N492"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="DEPARTMENT AML" queryTableFieldId="1" dataDxfId="147"/>
-    <tableColumn id="2" uniqueName="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" dataDxfId="146"/>
+    <tableColumn id="1" uniqueName="1" name="DEPARTMENT AML" queryTableFieldId="1" dataDxfId="53"/>
+    <tableColumn id="2" uniqueName="2" name="DEPARTMENT AML CODE" queryTableFieldId="2" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28063,7 +28101,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Query_Asset_User_Relationship_Personal" displayName="Query_Asset_User_Relationship_Personal" ref="CO1:CO14" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CO1:CO14"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Customer Relationship" queryTableFieldId="1" dataDxfId="107"/>
+    <tableColumn id="1" uniqueName="1" name="Customer Relationship" queryTableFieldId="1" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28073,7 +28111,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Query_Ownership_Code" displayName="Query_Ownership_Code" ref="CQ1:CQ8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CQ1:CQ8"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="OWNERSHIP CODE" queryTableFieldId="1" dataDxfId="106"/>
+    <tableColumn id="1" uniqueName="1" name="OWNERSHIP CODE" queryTableFieldId="1" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28083,7 +28121,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Query_Owner_Type" displayName="Query_Owner_Type" ref="CS1:CS3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CS1:CS3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Owner Type" queryTableFieldId="1" dataDxfId="105"/>
+    <tableColumn id="1" uniqueName="1" name="Owner Type" queryTableFieldId="1" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28093,7 +28131,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Query_Subsidy_From_Type" displayName="Query_Subsidy_From_Type" ref="CU1:CU6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CU1:CU6"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Subsidy From Type" queryTableFieldId="1" dataDxfId="104"/>
+    <tableColumn id="1" uniqueName="1" name="Subsidy From Type" queryTableFieldId="1" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28103,7 +28141,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Query_Subsidy_Allocation" displayName="Query_Subsidy_Allocation" ref="CW1:CW6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CW1:CW6"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Subsidy Allocation" queryTableFieldId="1" dataDxfId="103"/>
+    <tableColumn id="1" uniqueName="1" name="Subsidy Allocation" queryTableFieldId="1" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28113,7 +28151,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="45" name="Query_Subsidy_Source" displayName="Query_Subsidy_Source" ref="CY1:CY8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="CY1:CY8"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Subsidy Source" queryTableFieldId="1" dataDxfId="102"/>
+    <tableColumn id="1" uniqueName="1" name="Subsidy Source" queryTableFieldId="1" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28123,7 +28161,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Query_Provision_Calculation_Base" displayName="Query_Provision_Calculation_Base" ref="DA1:DA3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="DA1:DA3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Provision Calculation Base" queryTableFieldId="1" dataDxfId="101"/>
+    <tableColumn id="1" uniqueName="1" name="Provision Calculation Base" queryTableFieldId="1" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28133,7 +28171,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Query_Grace_Period_Type" displayName="Query_Grace_Period_Type" ref="DC1:DC3" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="DC1:DC3"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="Grace Period Type" queryTableFieldId="1" dataDxfId="100"/>
+    <tableColumn id="1" uniqueName="1" name="Grace Period Type" queryTableFieldId="1" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28154,8 +28192,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="Query_JobProfessionNonProfessional" displayName="Query_JobProfessionNonProfessional" ref="DJ1:DK6" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="DJ1:DK6"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION NONPROF" queryTableFieldId="1" dataDxfId="99"/>
-    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="98"/>
+    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION NONPROF" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28165,8 +28203,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="QueryAuthorityAML" displayName="QueryAuthorityAML" ref="Q1:R9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="Q1:R9"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="AUTHORITY AML" queryTableFieldId="1" dataDxfId="145"/>
-    <tableColumn id="2" uniqueName="2" name="AUTHORITY AML2" queryTableFieldId="2" dataDxfId="144"/>
+    <tableColumn id="1" uniqueName="1" name="AUTHORITY AML" queryTableFieldId="1" dataDxfId="51"/>
+    <tableColumn id="2" uniqueName="2" name="AUTHORITY AML2" queryTableFieldId="2" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28176,8 +28214,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="Query_JobProfessionSME" displayName="Query_JobProfessionSME" ref="DM1:DN15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="DM1:DN15"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION SME" queryTableFieldId="1" dataDxfId="97"/>
-    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="96"/>
+    <tableColumn id="1" uniqueName="1" name="JOB PROFESSION SME" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" uniqueName="2" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28187,8 +28225,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="_r3db_server_ad_ins_com\r3__LOS" displayName="_r3db_server_ad_ins_com\r3__LOS" ref="DP1:DQ94" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="DP1:DQ94"/>
   <tableColumns count="2">
-    <tableColumn id="7" uniqueName="7" name="JOB PROFESSION" queryTableFieldId="1" dataDxfId="95"/>
-    <tableColumn id="8" uniqueName="8" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="94"/>
+    <tableColumn id="7" uniqueName="7" name="JOB PROFESSION" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="8" uniqueName="8" name="JOB POSITION CODE" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28198,7 +28236,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="QueryIdType" displayName="QueryIdType" ref="T1:T15" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="T1:T15"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="ID TYPE" queryTableFieldId="1" dataDxfId="143"/>
+    <tableColumn id="1" uniqueName="1" name="ID TYPE" queryTableFieldId="1" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28208,7 +28246,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="QueryMaritalStatus" displayName="QueryMaritalStatus" ref="V1:V4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="V1:V4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="MARITAL STATUS" queryTableFieldId="1" dataDxfId="142"/>
+    <tableColumn id="1" uniqueName="1" name="MARITAL STATUS" queryTableFieldId="1" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28218,7 +28256,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="QueryNationality" displayName="QueryNationality" ref="X1:X4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="X1:X4"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="NATIONALITY" queryTableFieldId="1" dataDxfId="141"/>
+    <tableColumn id="1" uniqueName="1" name="NATIONALITY" queryTableFieldId="1" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28228,7 +28266,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="QueryOwnership" displayName="QueryOwnership" ref="Z1:Z8" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="Z1:Z8"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="OWNERSHIP" queryTableFieldId="1" dataDxfId="140"/>
+    <tableColumn id="1" uniqueName="1" name="OWNERSHIP" queryTableFieldId="1" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -28501,7 +28539,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28518,17 +28556,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
+      <c r="B1" s="18" t="s">
+        <v>3523</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3524</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>3525</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3526</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -28545,28 +28583,31 @@
         <f>COUNTA('1.TabCustomerMainData'!$B$12:$XFD$12)</f>
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3054</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3054</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3054</v>
+      <c r="B2" s="18">
+        <f>COUNTA('2.TabFamilyData'!$B$12:$XFD$12)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="18">
+        <f>COUNTA('3a.TabGuarantorDataPersonal'!$B$12:$XFD$12)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="18">
+        <f>COUNTA('3b.TabGuarantorDataCompany'!$B$12:$XFD$12)</f>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3054</v>
+        <v>3522</v>
       </c>
       <c r="F2" s="1">
-        <f>COUNTA('5.TabReferantorData'!B12:XFD12)</f>
+        <f>COUNTA('5.TabReferantorData'!$B$12:$XFD$12)</f>
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <f>COUNTA('7a.Accessories'!B12:XFD12)</f>
+        <f>COUNTA('7a.Accessories'!$B$12:$XFD$12)</f>
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <f>COUNTA('12.TabUploadDocument'!B12:XFD12)</f>
+        <f>COUNTA('12.TabUploadDocument'!$B$12:$XFD$12)</f>
         <v>4</v>
       </c>
     </row>
@@ -28656,14 +28697,14 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="122" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="120" t="s">
+    <row r="11" spans="1:5" s="123" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="121" t="s">
         <v>3026</v>
       </c>
-      <c r="B11" s="121"/>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
     </row>
     <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -28707,14 +28748,14 @@
         <v>3081</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="120" t="s">
+    <row r="16" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="121" t="s">
         <v>3027</v>
       </c>
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
     </row>
     <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
@@ -28913,11 +28954,11 @@
       </c>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="120" t="s">
+    <row r="34" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="121" t="s">
         <v>3028</v>
       </c>
-      <c r="B34" s="121"/>
+      <c r="B34" s="122"/>
     </row>
     <row r="35" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="58" t="s">
@@ -28930,11 +28971,11 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="120" t="s">
+    <row r="36" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="121" t="s">
         <v>3029</v>
       </c>
-      <c r="B36" s="121"/>
+      <c r="B36" s="122"/>
     </row>
     <row r="37" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -28969,11 +29010,11 @@
         <v>284</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="120" t="s">
+    <row r="40" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="121" t="s">
         <v>3030</v>
       </c>
-      <c r="B40" s="121"/>
+      <c r="B40" s="122"/>
     </row>
     <row r="41" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
@@ -29087,11 +29128,11 @@
         <v>1231413</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="120" t="s">
+    <row r="51" spans="1:8" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="121" t="s">
         <v>3425</v>
       </c>
-      <c r="B51" s="121"/>
+      <c r="B51" s="122"/>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
@@ -29192,11 +29233,11 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="120" t="s">
+    <row r="61" spans="1:8" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="121" t="s">
         <v>3086</v>
       </c>
-      <c r="B61" s="121"/>
+      <c r="B61" s="122"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="110" t="s">
@@ -29239,57 +29280,57 @@
     <mergeCell ref="A40:XFD40"/>
   </mergeCells>
   <conditionalFormatting sqref="A27:XFD27">
-    <cfRule type="expression" dxfId="59" priority="16">
+    <cfRule type="expression" dxfId="120" priority="16">
       <formula>A$26="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:XFD28">
-    <cfRule type="expression" dxfId="58" priority="15">
+    <cfRule type="expression" dxfId="119" priority="15">
       <formula>A$26="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:XFD39">
-    <cfRule type="expression" dxfId="57" priority="14">
+    <cfRule type="expression" dxfId="118" priority="14">
       <formula>A$37="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:XFD50">
-    <cfRule type="expression" dxfId="56" priority="13">
+    <cfRule type="expression" dxfId="117" priority="13">
       <formula>A$41="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A60 D54:XFD60">
-    <cfRule type="expression" dxfId="55" priority="10">
+    <cfRule type="expression" dxfId="116" priority="10">
       <formula>A$52="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:XFD53">
-    <cfRule type="expression" dxfId="54" priority="9">
+    <cfRule type="expression" dxfId="115" priority="9">
       <formula>A$52="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:XFD47">
-    <cfRule type="expression" dxfId="53" priority="8">
+    <cfRule type="expression" dxfId="114" priority="8">
       <formula>A$42="Personal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:XFD46">
-    <cfRule type="expression" dxfId="52" priority="7">
+    <cfRule type="expression" dxfId="113" priority="7">
       <formula>A$42="Company"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:XFD62">
-    <cfRule type="expression" dxfId="51" priority="6">
+    <cfRule type="expression" dxfId="112" priority="6">
       <formula>A$18="New"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:C60">
-    <cfRule type="expression" dxfId="50" priority="5">
+    <cfRule type="expression" dxfId="111" priority="5">
       <formula>B$41="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:C60">
-    <cfRule type="expression" dxfId="49" priority="4">
+    <cfRule type="expression" dxfId="110" priority="4">
       <formula>B$52="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29698,22 +29739,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19:XFD19">
-    <cfRule type="expression" dxfId="48" priority="6">
+    <cfRule type="expression" dxfId="109" priority="6">
       <formula>B$18="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:XFD20">
-    <cfRule type="expression" dxfId="47" priority="5">
+    <cfRule type="expression" dxfId="108" priority="5">
       <formula>B$18="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="107" priority="2">
       <formula>A$18="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="expression" dxfId="45" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>A$18="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29739,12 +29780,12 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="B79" sqref="B79"/>
+      <selection pane="topRight" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29760,7 +29801,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>9</v>
@@ -29776,8 +29817,8 @@
       <c r="A2" s="18" t="s">
         <v>3267</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>3054</v>
+      <c r="B2" t="s">
+        <v>3521</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3054</v>
@@ -29809,14 +29850,14 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="130" t="s">
+    <row r="11" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="131" t="s">
         <v>3031</v>
       </c>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
     </row>
     <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -29829,14 +29870,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="136" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="133" t="s">
+    <row r="13" spans="1:5" s="137" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="135"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="135"/>
+      <c r="D13" s="135"/>
+      <c r="E13" s="136"/>
     </row>
     <row r="14" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
@@ -29897,14 +29938,14 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="136" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="133" t="s">
+    <row r="21" spans="1:5" s="137" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="134"/>
-      <c r="C21" s="134"/>
-      <c r="D21" s="134"/>
-      <c r="E21" s="135"/>
+      <c r="B21" s="135"/>
+      <c r="C21" s="135"/>
+      <c r="D21" s="135"/>
+      <c r="E21" s="136"/>
     </row>
     <row r="22" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
@@ -29977,14 +30018,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="130" t="s">
+    <row r="29" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="131" t="s">
         <v>3032</v>
       </c>
-      <c r="B29" s="131"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="132"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
     </row>
     <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="64" t="s">
@@ -30019,14 +30060,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="140" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137" t="s">
+    <row r="33" spans="1:5" s="141" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="138" t="s">
         <v>3033</v>
       </c>
-      <c r="B33" s="138"/>
-      <c r="C33" s="138"/>
-      <c r="D33" s="138"/>
-      <c r="E33" s="139"/>
+      <c r="B33" s="139"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="139"/>
+      <c r="E33" s="140"/>
     </row>
     <row r="34" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="59" t="s">
@@ -30039,14 +30080,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="133" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="133" t="s">
+    <row r="35" spans="1:5" s="134" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="134" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="134"/>
-      <c r="C35" s="134"/>
-      <c r="D35" s="134"/>
-      <c r="E35" s="134"/>
+      <c r="B35" s="135"/>
+      <c r="C35" s="135"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="135"/>
     </row>
     <row r="36" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="s">
@@ -30138,14 +30179,14 @@
       <c r="D43" s="102"/>
       <c r="E43" s="102"/>
     </row>
-    <row r="44" spans="1:5" s="141" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="141" t="s">
+    <row r="44" spans="1:5" s="142" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="142" t="s">
         <v>3197</v>
       </c>
-      <c r="B44" s="142"/>
-      <c r="C44" s="142"/>
-      <c r="D44" s="142"/>
-      <c r="E44" s="142"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="143"/>
+      <c r="D44" s="143"/>
+      <c r="E44" s="143"/>
     </row>
     <row r="45" spans="1:5" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="90" t="s">
@@ -30163,7 +30204,7 @@
         <v>3171</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>3184</v>
+        <v>3527</v>
       </c>
       <c r="C46" s="91" t="s">
         <v>3184</v>
@@ -30191,14 +30232,14 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="143" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="143" t="s">
+    <row r="49" spans="1:5" s="144" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="144" t="s">
         <v>128</v>
       </c>
-      <c r="B49" s="144"/>
-      <c r="C49" s="144"/>
-      <c r="D49" s="144"/>
-      <c r="E49" s="144"/>
+      <c r="B49" s="145"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145"/>
     </row>
     <row r="50" spans="1:5" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="90" t="s">
@@ -30288,8 +30329,8 @@
         <v>3188</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="145" t="s">
+    <row r="58" spans="1:5" s="146" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="146" t="s">
         <v>3173</v>
       </c>
     </row>
@@ -30503,11 +30544,11 @@
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
     </row>
-    <row r="80" spans="1:3" s="128" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="128" t="s">
+    <row r="80" spans="1:3" s="129" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="129" t="s">
         <v>3034</v>
       </c>
-      <c r="B80" s="129"/>
+      <c r="B80" s="130"/>
     </row>
     <row r="81" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
@@ -30525,57 +30566,79 @@
         <v>3193</v>
       </c>
       <c r="B82" t="s">
-        <v>3516</v>
+        <v>3528</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>3306</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="124" t="s">
+    <row r="83" spans="1:3" s="105" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="112" t="s">
+        <v>3518</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>3519</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>3520</v>
+      </c>
+      <c r="B85" s="18">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="125" t="s">
         <v>3182</v>
       </c>
-      <c r="B84" s="125"/>
-    </row>
-    <row r="85" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="96" t="s">
+      <c r="B87" s="126"/>
+    </row>
+    <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="96" t="s">
         <v>3195</v>
       </c>
-      <c r="B85" s="97">
+      <c r="B88" s="97">
         <f>IF(B24="Annualy",0,IF(B24="Full Tenor",ROUNDUP('6.TabApplicationData'!B20/12,0)-1,ROUNDUP(B28/12,0)-1))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="126" t="s">
+    <row r="89" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="127" t="s">
         <v>3181</v>
       </c>
-      <c r="B86" s="127"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="89" t="s">
+      <c r="B89" s="128"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="89" t="s">
         <v>3196</v>
       </c>
-      <c r="B87" s="97">
-        <f>B85+1</f>
+      <c r="B90" s="97">
+        <f>B88+1</f>
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="123" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="124" t="s">
         <v>3201</v>
       </c>
-      <c r="B88" s="123"/>
-    </row>
-    <row r="89" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="123"/>
-      <c r="B89" s="123"/>
+      <c r="B91" s="124"/>
+    </row>
+    <row r="92" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="124"/>
+      <c r="B92" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A88:B89"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A91:B92"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A89:B89"/>
     <mergeCell ref="A80:XFD80"/>
     <mergeCell ref="A11:XFD11"/>
     <mergeCell ref="A13:XFD13"/>
@@ -30588,91 +30651,96 @@
     <mergeCell ref="A58:XFD58"/>
   </mergeCells>
   <conditionalFormatting sqref="B28:XFD28">
-    <cfRule type="expression" dxfId="44" priority="19">
+    <cfRule type="expression" dxfId="105" priority="20">
       <formula>OR(B$24="Annualy",B$24="Full Tenor")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35 A44 A49 A58 D74:XFD78 B59:B71 A68:A71 A72:B73 A45:XFD48 A50:XFD57 C59:C66 C69 C71:C73 A79:C79 A81:XFD82 B22:XFD28 A30:XFD32 B34:XFD34 B36:XFD43">
-    <cfRule type="expression" dxfId="43" priority="18">
+    <cfRule type="expression" dxfId="104" priority="19">
       <formula>A$12="Customer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35 A44 A49 A58 D74:XFD78 B59:B71 A68:A71 A72:B73 B14:XFD20 A45:XFD48 A50:XFD57 C59:C66 C69 C71:C73 A79:C79 A81:XFD82 B22:XFD28 A30:XFD32 B34:XFD34 B36:XFD43">
-    <cfRule type="expression" dxfId="42" priority="17">
+    <cfRule type="expression" dxfId="103" priority="18">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:XFD20">
-    <cfRule type="expression" dxfId="41" priority="16">
+    <cfRule type="expression" dxfId="102" priority="17">
       <formula>B$12="Multifinance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:XFD32">
-    <cfRule type="expression" dxfId="40" priority="15">
+    <cfRule type="expression" dxfId="101" priority="16">
       <formula>A$30="YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A66">
-    <cfRule type="expression" dxfId="39" priority="14">
+    <cfRule type="expression" dxfId="100" priority="15">
       <formula>A$12="Customer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A66">
-    <cfRule type="expression" dxfId="38" priority="13">
+    <cfRule type="expression" dxfId="99" priority="14">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:XFD82">
-    <cfRule type="expression" dxfId="37" priority="10">
+    <cfRule type="expression" dxfId="98" priority="11">
       <formula>A$82="Discount Amount (Paid By MF)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A20">
-    <cfRule type="expression" dxfId="36" priority="9">
+    <cfRule type="expression" dxfId="97" priority="10">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A20">
-    <cfRule type="expression" dxfId="35" priority="8">
+    <cfRule type="expression" dxfId="96" priority="9">
       <formula>A$12="Multifinance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="34" priority="7">
+    <cfRule type="expression" dxfId="95" priority="8">
       <formula>OR(A$24="Annualy",A$24="Full Tenor")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A28">
-    <cfRule type="expression" dxfId="33" priority="6">
+    <cfRule type="expression" dxfId="94" priority="7">
       <formula>A$12="Customer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A28">
-    <cfRule type="expression" dxfId="32" priority="5">
+    <cfRule type="expression" dxfId="93" priority="6">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="92" priority="5">
       <formula>A$12="Customer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="30" priority="3">
+    <cfRule type="expression" dxfId="91" priority="4">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:A43">
-    <cfRule type="expression" dxfId="29" priority="2">
+    <cfRule type="expression" dxfId="90" priority="3">
       <formula>A$12="Customer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:A43">
-    <cfRule type="expression" dxfId="28" priority="1">
+    <cfRule type="expression" dxfId="89" priority="2">
       <formula>A$12="Off System"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="15">
+  <conditionalFormatting sqref="A85:XFD85">
+    <cfRule type="expression" dxfId="88" priority="1">
+      <formula>A$84="YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="14">
     <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31:C31">
       <formula1>AND(OR(B$12="Multifinance",B$12="Customer - Multifinance"),B30="NO",ISNUMBER(B31))</formula1>
     </dataValidation>
@@ -30682,13 +30750,13 @@
     <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:C28">
       <formula1>AND(OR(B$12="Multifinance",B$12="Customer - Multifinance"),B24&lt;&gt;"Annualy",B24&lt;&gt;"Full Tenor",ISNUMBER(B28))</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:C82">
-      <formula1>AND(OR(B$12="Multifinance",B$12="Customer - Multifinance"),ISNUMBER(B82))</formula1>
+    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:C23 B81:C82">
+      <formula1>AND(OR(B$12="Multifinance",B$12="Customer - Multifinance"),ISNUMBER(B23))</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:C12">
       <formula1>ListInsuredBy</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:C20">
+    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:C14 B16:C20">
       <formula1>OR(B$12="Customer", B$12="Customer - Multifinance")</formula1>
     </dataValidation>
     <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:C15">
@@ -30696,12 +30764,6 @@
     </dataValidation>
     <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27:C27">
       <formula1>OR(B$12="Multifinance",B$12="Customer - Multifinance")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:C14 B16:C19">
-      <formula1>OR(B$12="Customer", B$12="Customer - Multifinance")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:C23 B81:C81">
-      <formula1>AND(OR(B$12="Multifinance",B$12="Customer - Multifinance"),ISNUMBER(B23))</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:C22">
       <formula1>ListAssetRegion</formula1>
@@ -30717,6 +30779,9 @@
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:C34">
       <formula1>ListInsMainCoverage</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84">
+      <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30810,8 +30875,8 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112" t="s">
+    <row r="11" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="113" t="s">
         <v>3035</v>
       </c>
     </row>
@@ -30864,8 +30929,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="112" t="s">
+    <row r="17" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="113" t="s">
         <v>3036</v>
       </c>
     </row>
@@ -30913,8 +30978,8 @@
         <v>2451</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112" t="s">
+    <row r="22" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="113" t="s">
         <v>3037</v>
       </c>
     </row>
@@ -30940,42 +31005,42 @@
     <mergeCell ref="A22:XFD22"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:XFD23 A16:XFD16 B18:XFD21 B13:XFD15">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="87" priority="8">
       <formula>A$12="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:XFD15">
-    <cfRule type="expression" dxfId="26" priority="7">
+    <cfRule type="expression" dxfId="86" priority="7">
       <formula>AND(B$14&lt;&gt;"Paid in Advance &amp; Capitalized Mix",B$14&lt;&gt;"",B$14&lt;&gt;"Premium Payment Method")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:XFD21">
-    <cfRule type="expression" dxfId="25" priority="6">
+    <cfRule type="expression" dxfId="85" priority="6">
       <formula>AND(B$19&lt;&gt;"YES PARTIAL",B$19&lt;&gt;"",B$19&lt;&gt;"Subject Guarantor")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:A15">
-    <cfRule type="expression" dxfId="24" priority="5">
+    <cfRule type="expression" dxfId="84" priority="5">
       <formula>A$12="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="83" priority="4">
       <formula>AND(A$14&lt;&gt;"Paid in Advance &amp; Capitalized Mix",A$14&lt;&gt;"",A$14&lt;&gt;"Premium Payment Method")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:A21">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="82" priority="3">
       <formula>A$12="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>AND(A$19&lt;&gt;"YES PARTIAL",A$19&lt;&gt;"",A$19&lt;&gt;"Subject Guarantor")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="80" priority="1">
       <formula>A$12="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31097,14 +31162,14 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="130" t="s">
+    <row r="11" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="131" t="s">
         <v>3038</v>
       </c>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
     </row>
     <row r="12" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
@@ -31165,14 +31230,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="130" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="130" t="s">
+    <row r="19" spans="1:5" s="131" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="131" t="s">
         <v>3039</v>
       </c>
-      <c r="B19" s="131"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="131"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
     </row>
     <row r="20" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
@@ -31416,14 +31481,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="130" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="130" t="s">
+    <row r="42" spans="1:5" s="131" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="131" t="s">
         <v>3040</v>
       </c>
-      <c r="B42" s="131"/>
-      <c r="C42" s="131"/>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131"/>
+      <c r="B42" s="132"/>
+      <c r="C42" s="132"/>
+      <c r="D42" s="132"/>
+      <c r="E42" s="132"/>
     </row>
     <row r="43" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -31520,77 +31585,77 @@
     <mergeCell ref="A42:XFD42"/>
   </mergeCells>
   <conditionalFormatting sqref="A21:XFD41">
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="79" priority="22">
       <formula>A$20="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:XFD35">
-    <cfRule type="expression" dxfId="18" priority="17">
+    <cfRule type="expression" dxfId="78" priority="17">
       <formula>A$34="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:XFD27">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="77" priority="21">
       <formula>A$26="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:XFD29">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="76" priority="20">
       <formula>A$28="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:XFD31">
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="75" priority="19">
       <formula>A$30="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:XFD33">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="74" priority="18">
       <formula>A$32="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:XFD38">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="73" priority="16">
       <formula>A$36="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:XFD39">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="72" priority="15">
       <formula>A$36="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:XFD41">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="71" priority="14">
       <formula>A$40="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:XFD45">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="70" priority="13">
       <formula>A$43="Effective Rate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:XFD44">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="69" priority="12">
       <formula>A$43="Flat Rate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:XFD48">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="68" priority="9">
       <formula>B$46="No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="67" priority="4">
       <formula>#REF!="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="66" priority="3">
       <formula>#REF!="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A48">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="65" priority="1">
       <formula>A$46="No"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31862,10 +31927,10 @@
       <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" s="25" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="146" t="s">
+      <c r="A20" s="147" t="s">
         <v>2453</v>
       </c>
-      <c r="B20" s="146"/>
+      <c r="B20" s="147"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -32154,14 +32219,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="128" t="s">
+    <row r="13" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="129" t="s">
         <v>2443</v>
       </c>
-      <c r="B13" s="129"/>
-      <c r="C13" s="129"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="147"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="148"/>
     </row>
     <row r="14" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -32349,14 +32414,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="128" t="s">
+    <row r="26" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="129" t="s">
         <v>2447</v>
       </c>
-      <c r="B26" s="129"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="147"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="148"/>
     </row>
     <row r="27" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -32595,11 +32660,11 @@
         <v>3337</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="128" t="s">
+    <row r="42" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="129" t="s">
         <v>2436</v>
       </c>
-      <c r="B42" s="129"/>
+      <c r="B42" s="130"/>
     </row>
     <row r="43" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -32740,10 +32805,10 @@
       <c r="B54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="149" t="s">
+      <c r="A55" s="150" t="s">
         <v>2440</v>
       </c>
-      <c r="B55" s="150"/>
+      <c r="B55" s="151"/>
     </row>
     <row r="56" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
@@ -32769,12 +32834,12 @@
     <mergeCell ref="A55:B55"/>
   </mergeCells>
   <conditionalFormatting sqref="A17:XFD17 A19:XFD19 A21:XFD21 A23:XFD23 A25:XFD25 A31:XFD31 A33:XFD33 A35:XFD35 A37:XFD37 A39:XFD39 A41:XFD41 A46:XFD46 A48:XFD48 A50:XFD50 A52:XFD52">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>A$12="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:XFD16 A18:XFD18 A20:XFD20 A22:XFD22 A24:XFD24 A30:XFD30 A32:XFD32 A34:XFD34 A38:XFD38 A40:XFD40 A36:XFD36 A45:XFD45 A47:XFD47 A49:XFD49 A51:XFD51">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="60" priority="1">
       <formula>A$12="Percentage"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33326,7 +33391,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>3517</v>
+        <v>3516</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13"/>
@@ -33353,8 +33418,8 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="112" t="s">
+    <row r="15" spans="1:13" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="113" t="s">
         <v>3015</v>
       </c>
     </row>
@@ -33663,8 +33728,8 @@
         <v>3215</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="112" t="s">
+    <row r="32" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="113" t="s">
         <v>3016</v>
       </c>
     </row>
@@ -33746,8 +33811,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="112" t="s">
+    <row r="37" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="113" t="s">
         <v>3017</v>
       </c>
     </row>
@@ -33943,17 +34008,17 @@
     <mergeCell ref="A37:XFD37"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:XFD18">
-    <cfRule type="expression" dxfId="93" priority="3">
+    <cfRule type="expression" dxfId="154" priority="3">
       <formula>A$14="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31 G26:XFD31 A19:XFD24 A26:F30 A38:XFD45">
-    <cfRule type="expression" dxfId="92" priority="2">
+    <cfRule type="expression" dxfId="153" priority="2">
       <formula>A$14="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:XFD22">
-    <cfRule type="expression" dxfId="91" priority="1">
+    <cfRule type="expression" dxfId="152" priority="1">
       <formula>OR(A$21="E-KTP",A$21="AKTA",A$21="NPWP")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46490,110 +46555,110 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="40" spans="1:101" s="116" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="113" t="s">
+    <row r="40" spans="1:101" s="117" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="114" t="s">
         <v>3016</v>
       </c>
-      <c r="B40" s="114"/>
-      <c r="C40" s="114"/>
-      <c r="D40" s="114"/>
-      <c r="E40" s="114"/>
-      <c r="F40" s="114"/>
-      <c r="G40" s="114"/>
-      <c r="H40" s="114"/>
-      <c r="I40" s="114"/>
-      <c r="J40" s="114"/>
-      <c r="K40" s="114"/>
-      <c r="L40" s="114"/>
-      <c r="M40" s="114"/>
-      <c r="N40" s="114"/>
-      <c r="O40" s="114"/>
-      <c r="P40" s="114"/>
-      <c r="Q40" s="114"/>
-      <c r="R40" s="114"/>
-      <c r="S40" s="114"/>
-      <c r="T40" s="114"/>
-      <c r="U40" s="114"/>
-      <c r="V40" s="114"/>
-      <c r="W40" s="114"/>
-      <c r="X40" s="114"/>
-      <c r="Y40" s="114"/>
-      <c r="Z40" s="114"/>
-      <c r="AA40" s="114"/>
-      <c r="AB40" s="114"/>
-      <c r="AC40" s="114"/>
-      <c r="AD40" s="114"/>
-      <c r="AE40" s="114"/>
-      <c r="AF40" s="114"/>
-      <c r="AG40" s="114"/>
-      <c r="AH40" s="114"/>
-      <c r="AI40" s="114"/>
-      <c r="AJ40" s="114"/>
-      <c r="AK40" s="114"/>
-      <c r="AL40" s="114"/>
-      <c r="AM40" s="114"/>
-      <c r="AN40" s="114"/>
-      <c r="AO40" s="114"/>
-      <c r="AP40" s="114"/>
-      <c r="AQ40" s="114"/>
-      <c r="AR40" s="114"/>
-      <c r="AS40" s="114"/>
-      <c r="AT40" s="114"/>
-      <c r="AU40" s="114"/>
-      <c r="AV40" s="114"/>
-      <c r="AW40" s="114"/>
-      <c r="AX40" s="114"/>
-      <c r="AY40" s="114"/>
-      <c r="AZ40" s="114"/>
-      <c r="BA40" s="114"/>
-      <c r="BB40" s="114"/>
-      <c r="BC40" s="114"/>
-      <c r="BD40" s="114"/>
-      <c r="BE40" s="114"/>
-      <c r="BF40" s="114"/>
-      <c r="BG40" s="114"/>
-      <c r="BH40" s="114"/>
-      <c r="BI40" s="114"/>
-      <c r="BJ40" s="114"/>
-      <c r="BK40" s="114"/>
-      <c r="BL40" s="114"/>
-      <c r="BM40" s="114"/>
-      <c r="BN40" s="114"/>
-      <c r="BO40" s="114"/>
-      <c r="BP40" s="114"/>
-      <c r="BQ40" s="114"/>
-      <c r="BR40" s="114"/>
-      <c r="BS40" s="114"/>
-      <c r="BT40" s="114"/>
-      <c r="BU40" s="114"/>
-      <c r="BV40" s="114"/>
-      <c r="BW40" s="114"/>
-      <c r="BX40" s="114"/>
-      <c r="BY40" s="114"/>
-      <c r="BZ40" s="114"/>
-      <c r="CA40" s="114"/>
-      <c r="CB40" s="114"/>
-      <c r="CC40" s="114"/>
-      <c r="CD40" s="114"/>
-      <c r="CE40" s="114"/>
-      <c r="CF40" s="114"/>
-      <c r="CG40" s="114"/>
-      <c r="CH40" s="114"/>
-      <c r="CI40" s="114"/>
-      <c r="CJ40" s="114"/>
-      <c r="CK40" s="114"/>
-      <c r="CL40" s="114"/>
-      <c r="CM40" s="114"/>
-      <c r="CN40" s="114"/>
-      <c r="CO40" s="114"/>
-      <c r="CP40" s="114"/>
-      <c r="CQ40" s="114"/>
-      <c r="CR40" s="114"/>
-      <c r="CS40" s="114"/>
-      <c r="CT40" s="114"/>
-      <c r="CU40" s="114"/>
-      <c r="CV40" s="114"/>
-      <c r="CW40" s="115"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="115"/>
+      <c r="H40" s="115"/>
+      <c r="I40" s="115"/>
+      <c r="J40" s="115"/>
+      <c r="K40" s="115"/>
+      <c r="L40" s="115"/>
+      <c r="M40" s="115"/>
+      <c r="N40" s="115"/>
+      <c r="O40" s="115"/>
+      <c r="P40" s="115"/>
+      <c r="Q40" s="115"/>
+      <c r="R40" s="115"/>
+      <c r="S40" s="115"/>
+      <c r="T40" s="115"/>
+      <c r="U40" s="115"/>
+      <c r="V40" s="115"/>
+      <c r="W40" s="115"/>
+      <c r="X40" s="115"/>
+      <c r="Y40" s="115"/>
+      <c r="Z40" s="115"/>
+      <c r="AA40" s="115"/>
+      <c r="AB40" s="115"/>
+      <c r="AC40" s="115"/>
+      <c r="AD40" s="115"/>
+      <c r="AE40" s="115"/>
+      <c r="AF40" s="115"/>
+      <c r="AG40" s="115"/>
+      <c r="AH40" s="115"/>
+      <c r="AI40" s="115"/>
+      <c r="AJ40" s="115"/>
+      <c r="AK40" s="115"/>
+      <c r="AL40" s="115"/>
+      <c r="AM40" s="115"/>
+      <c r="AN40" s="115"/>
+      <c r="AO40" s="115"/>
+      <c r="AP40" s="115"/>
+      <c r="AQ40" s="115"/>
+      <c r="AR40" s="115"/>
+      <c r="AS40" s="115"/>
+      <c r="AT40" s="115"/>
+      <c r="AU40" s="115"/>
+      <c r="AV40" s="115"/>
+      <c r="AW40" s="115"/>
+      <c r="AX40" s="115"/>
+      <c r="AY40" s="115"/>
+      <c r="AZ40" s="115"/>
+      <c r="BA40" s="115"/>
+      <c r="BB40" s="115"/>
+      <c r="BC40" s="115"/>
+      <c r="BD40" s="115"/>
+      <c r="BE40" s="115"/>
+      <c r="BF40" s="115"/>
+      <c r="BG40" s="115"/>
+      <c r="BH40" s="115"/>
+      <c r="BI40" s="115"/>
+      <c r="BJ40" s="115"/>
+      <c r="BK40" s="115"/>
+      <c r="BL40" s="115"/>
+      <c r="BM40" s="115"/>
+      <c r="BN40" s="115"/>
+      <c r="BO40" s="115"/>
+      <c r="BP40" s="115"/>
+      <c r="BQ40" s="115"/>
+      <c r="BR40" s="115"/>
+      <c r="BS40" s="115"/>
+      <c r="BT40" s="115"/>
+      <c r="BU40" s="115"/>
+      <c r="BV40" s="115"/>
+      <c r="BW40" s="115"/>
+      <c r="BX40" s="115"/>
+      <c r="BY40" s="115"/>
+      <c r="BZ40" s="115"/>
+      <c r="CA40" s="115"/>
+      <c r="CB40" s="115"/>
+      <c r="CC40" s="115"/>
+      <c r="CD40" s="115"/>
+      <c r="CE40" s="115"/>
+      <c r="CF40" s="115"/>
+      <c r="CG40" s="115"/>
+      <c r="CH40" s="115"/>
+      <c r="CI40" s="115"/>
+      <c r="CJ40" s="115"/>
+      <c r="CK40" s="115"/>
+      <c r="CL40" s="115"/>
+      <c r="CM40" s="115"/>
+      <c r="CN40" s="115"/>
+      <c r="CO40" s="115"/>
+      <c r="CP40" s="115"/>
+      <c r="CQ40" s="115"/>
+      <c r="CR40" s="115"/>
+      <c r="CS40" s="115"/>
+      <c r="CT40" s="115"/>
+      <c r="CU40" s="115"/>
+      <c r="CV40" s="115"/>
+      <c r="CW40" s="116"/>
     </row>
     <row r="41" spans="1:101" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="61" t="s">
@@ -46676,110 +46741,110 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:101" s="113" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="113" t="s">
+    <row r="45" spans="1:101" s="114" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="114" t="s">
         <v>3017</v>
       </c>
-      <c r="B45" s="114"/>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-      <c r="G45" s="114"/>
-      <c r="H45" s="114"/>
-      <c r="I45" s="114"/>
-      <c r="J45" s="114"/>
-      <c r="K45" s="114"/>
-      <c r="L45" s="114"/>
-      <c r="M45" s="114"/>
-      <c r="N45" s="114"/>
-      <c r="O45" s="114"/>
-      <c r="P45" s="114"/>
-      <c r="Q45" s="114"/>
-      <c r="R45" s="114"/>
-      <c r="S45" s="114"/>
-      <c r="T45" s="114"/>
-      <c r="U45" s="114"/>
-      <c r="V45" s="114"/>
-      <c r="W45" s="114"/>
-      <c r="X45" s="114"/>
-      <c r="Y45" s="114"/>
-      <c r="Z45" s="114"/>
-      <c r="AA45" s="114"/>
-      <c r="AB45" s="114"/>
-      <c r="AC45" s="114"/>
-      <c r="AD45" s="114"/>
-      <c r="AE45" s="114"/>
-      <c r="AF45" s="114"/>
-      <c r="AG45" s="114"/>
-      <c r="AH45" s="114"/>
-      <c r="AI45" s="114"/>
-      <c r="AJ45" s="114"/>
-      <c r="AK45" s="114"/>
-      <c r="AL45" s="114"/>
-      <c r="AM45" s="114"/>
-      <c r="AN45" s="114"/>
-      <c r="AO45" s="114"/>
-      <c r="AP45" s="114"/>
-      <c r="AQ45" s="114"/>
-      <c r="AR45" s="114"/>
-      <c r="AS45" s="114"/>
-      <c r="AT45" s="114"/>
-      <c r="AU45" s="114"/>
-      <c r="AV45" s="114"/>
-      <c r="AW45" s="114"/>
-      <c r="AX45" s="114"/>
-      <c r="AY45" s="114"/>
-      <c r="AZ45" s="114"/>
-      <c r="BA45" s="114"/>
-      <c r="BB45" s="114"/>
-      <c r="BC45" s="114"/>
-      <c r="BD45" s="114"/>
-      <c r="BE45" s="114"/>
-      <c r="BF45" s="114"/>
-      <c r="BG45" s="114"/>
-      <c r="BH45" s="114"/>
-      <c r="BI45" s="114"/>
-      <c r="BJ45" s="114"/>
-      <c r="BK45" s="114"/>
-      <c r="BL45" s="114"/>
-      <c r="BM45" s="114"/>
-      <c r="BN45" s="114"/>
-      <c r="BO45" s="114"/>
-      <c r="BP45" s="114"/>
-      <c r="BQ45" s="114"/>
-      <c r="BR45" s="114"/>
-      <c r="BS45" s="114"/>
-      <c r="BT45" s="114"/>
-      <c r="BU45" s="114"/>
-      <c r="BV45" s="114"/>
-      <c r="BW45" s="114"/>
-      <c r="BX45" s="114"/>
-      <c r="BY45" s="114"/>
-      <c r="BZ45" s="114"/>
-      <c r="CA45" s="114"/>
-      <c r="CB45" s="114"/>
-      <c r="CC45" s="114"/>
-      <c r="CD45" s="114"/>
-      <c r="CE45" s="114"/>
-      <c r="CF45" s="114"/>
-      <c r="CG45" s="114"/>
-      <c r="CH45" s="114"/>
-      <c r="CI45" s="114"/>
-      <c r="CJ45" s="114"/>
-      <c r="CK45" s="114"/>
-      <c r="CL45" s="114"/>
-      <c r="CM45" s="114"/>
-      <c r="CN45" s="114"/>
-      <c r="CO45" s="114"/>
-      <c r="CP45" s="114"/>
-      <c r="CQ45" s="114"/>
-      <c r="CR45" s="114"/>
-      <c r="CS45" s="114"/>
-      <c r="CT45" s="114"/>
-      <c r="CU45" s="114"/>
-      <c r="CV45" s="114"/>
-      <c r="CW45" s="114"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="115"/>
+      <c r="J45" s="115"/>
+      <c r="K45" s="115"/>
+      <c r="L45" s="115"/>
+      <c r="M45" s="115"/>
+      <c r="N45" s="115"/>
+      <c r="O45" s="115"/>
+      <c r="P45" s="115"/>
+      <c r="Q45" s="115"/>
+      <c r="R45" s="115"/>
+      <c r="S45" s="115"/>
+      <c r="T45" s="115"/>
+      <c r="U45" s="115"/>
+      <c r="V45" s="115"/>
+      <c r="W45" s="115"/>
+      <c r="X45" s="115"/>
+      <c r="Y45" s="115"/>
+      <c r="Z45" s="115"/>
+      <c r="AA45" s="115"/>
+      <c r="AB45" s="115"/>
+      <c r="AC45" s="115"/>
+      <c r="AD45" s="115"/>
+      <c r="AE45" s="115"/>
+      <c r="AF45" s="115"/>
+      <c r="AG45" s="115"/>
+      <c r="AH45" s="115"/>
+      <c r="AI45" s="115"/>
+      <c r="AJ45" s="115"/>
+      <c r="AK45" s="115"/>
+      <c r="AL45" s="115"/>
+      <c r="AM45" s="115"/>
+      <c r="AN45" s="115"/>
+      <c r="AO45" s="115"/>
+      <c r="AP45" s="115"/>
+      <c r="AQ45" s="115"/>
+      <c r="AR45" s="115"/>
+      <c r="AS45" s="115"/>
+      <c r="AT45" s="115"/>
+      <c r="AU45" s="115"/>
+      <c r="AV45" s="115"/>
+      <c r="AW45" s="115"/>
+      <c r="AX45" s="115"/>
+      <c r="AY45" s="115"/>
+      <c r="AZ45" s="115"/>
+      <c r="BA45" s="115"/>
+      <c r="BB45" s="115"/>
+      <c r="BC45" s="115"/>
+      <c r="BD45" s="115"/>
+      <c r="BE45" s="115"/>
+      <c r="BF45" s="115"/>
+      <c r="BG45" s="115"/>
+      <c r="BH45" s="115"/>
+      <c r="BI45" s="115"/>
+      <c r="BJ45" s="115"/>
+      <c r="BK45" s="115"/>
+      <c r="BL45" s="115"/>
+      <c r="BM45" s="115"/>
+      <c r="BN45" s="115"/>
+      <c r="BO45" s="115"/>
+      <c r="BP45" s="115"/>
+      <c r="BQ45" s="115"/>
+      <c r="BR45" s="115"/>
+      <c r="BS45" s="115"/>
+      <c r="BT45" s="115"/>
+      <c r="BU45" s="115"/>
+      <c r="BV45" s="115"/>
+      <c r="BW45" s="115"/>
+      <c r="BX45" s="115"/>
+      <c r="BY45" s="115"/>
+      <c r="BZ45" s="115"/>
+      <c r="CA45" s="115"/>
+      <c r="CB45" s="115"/>
+      <c r="CC45" s="115"/>
+      <c r="CD45" s="115"/>
+      <c r="CE45" s="115"/>
+      <c r="CF45" s="115"/>
+      <c r="CG45" s="115"/>
+      <c r="CH45" s="115"/>
+      <c r="CI45" s="115"/>
+      <c r="CJ45" s="115"/>
+      <c r="CK45" s="115"/>
+      <c r="CL45" s="115"/>
+      <c r="CM45" s="115"/>
+      <c r="CN45" s="115"/>
+      <c r="CO45" s="115"/>
+      <c r="CP45" s="115"/>
+      <c r="CQ45" s="115"/>
+      <c r="CR45" s="115"/>
+      <c r="CS45" s="115"/>
+      <c r="CT45" s="115"/>
+      <c r="CU45" s="115"/>
+      <c r="CV45" s="115"/>
+      <c r="CW45" s="115"/>
     </row>
     <row r="46" spans="1:101" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -47245,16 +47310,16 @@
       </c>
     </row>
     <row r="60" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="117" t="s">
+      <c r="A60" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="117" t="s">
+      <c r="B60" s="118" t="s">
         <v>3160</v>
       </c>
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A61" s="118"/>
-      <c r="B61" s="118"/>
+      <c r="A61" s="119"/>
+      <c r="B61" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -47264,32 +47329,32 @@
     <mergeCell ref="A60:A61"/>
   </mergeCells>
   <conditionalFormatting sqref="A15:XFD17">
-    <cfRule type="expression" dxfId="90" priority="8">
+    <cfRule type="expression" dxfId="151" priority="8">
       <formula>A$13="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32 G29:XFD34 A33:F34 A19:XFD24 A29:F30 A46:XFD54">
-    <cfRule type="expression" dxfId="89" priority="7">
+    <cfRule type="expression" dxfId="150" priority="7">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:XFD22">
-    <cfRule type="expression" dxfId="88" priority="4">
+    <cfRule type="expression" dxfId="149" priority="4">
       <formula>OR(A$21="E-KTP",A$21="AKTA",A$21="NPWP")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:XFD37">
-    <cfRule type="expression" dxfId="87" priority="3">
+    <cfRule type="expression" dxfId="148" priority="3">
       <formula>AND(A$35&lt;&gt;"Foreigner",A$35&lt;&gt;"Nationality",A$35&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:XFD54">
-    <cfRule type="expression" dxfId="86" priority="2">
+    <cfRule type="expression" dxfId="147" priority="2">
       <formula>A$46="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:F32">
-    <cfRule type="expression" dxfId="85" priority="1">
+    <cfRule type="expression" dxfId="146" priority="1">
       <formula>B$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47432,7 +47497,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -47589,10 +47654,10 @@
       <c r="A14" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="120" t="s">
         <v>3161</v>
       </c>
-      <c r="C14" s="119"/>
+      <c r="C14" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -47607,7 +47672,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
@@ -47726,8 +47791,8 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112" t="s">
+    <row r="14" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
         <v>3020</v>
       </c>
     </row>
@@ -48031,8 +48096,8 @@
         <v>3226</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="112" t="s">
+    <row r="32" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="113" t="s">
         <v>3016</v>
       </c>
     </row>
@@ -48126,8 +48191,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="112" t="s">
+    <row r="37" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="113" t="s">
         <v>3017</v>
       </c>
     </row>
@@ -48315,47 +48380,47 @@
     <mergeCell ref="A14:XFD14"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:XFD17">
-    <cfRule type="expression" dxfId="84" priority="9">
+    <cfRule type="expression" dxfId="145" priority="9">
       <formula>B$13="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:XFD24 B26:XFD31 A38:XFD38 B39:XFD46">
-    <cfRule type="expression" dxfId="83" priority="8">
+    <cfRule type="expression" dxfId="144" priority="8">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:XFD22">
-    <cfRule type="expression" dxfId="82" priority="7">
+    <cfRule type="expression" dxfId="143" priority="7">
       <formula>OR(B$21="E-KTP",B$21="AKTA",B$21="NPWP")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:XFD46">
-    <cfRule type="expression" dxfId="81" priority="6">
+    <cfRule type="expression" dxfId="142" priority="6">
       <formula>B$38="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A17">
-    <cfRule type="expression" dxfId="80" priority="5">
+    <cfRule type="expression" dxfId="141" priority="5">
       <formula>A$13="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A24 A26:A31">
-    <cfRule type="expression" dxfId="79" priority="4">
+    <cfRule type="expression" dxfId="140" priority="4">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="78" priority="3">
+    <cfRule type="expression" dxfId="139" priority="3">
       <formula>OR(A$21="E-KTP",A$21="AKTA",A$21="NPWP")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A46">
-    <cfRule type="expression" dxfId="77" priority="2">
+    <cfRule type="expression" dxfId="138" priority="2">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A46">
-    <cfRule type="expression" dxfId="76" priority="1">
+    <cfRule type="expression" dxfId="137" priority="1">
       <formula>A$38="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48595,8 +48660,8 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112" t="s">
+    <row r="14" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="113" t="s">
         <v>3020</v>
       </c>
     </row>
@@ -48720,8 +48785,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="112" t="s">
+    <row r="22" spans="1:6" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="113" t="s">
         <v>3017</v>
       </c>
     </row>
@@ -48908,37 +48973,37 @@
     <mergeCell ref="A22:XFD22"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:XFD16">
-    <cfRule type="expression" dxfId="75" priority="7">
+    <cfRule type="expression" dxfId="136" priority="7">
       <formula>B$13="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:XFD19 B21:XFD21 A23:XFD23 B24:XFD31">
-    <cfRule type="expression" dxfId="74" priority="6">
+    <cfRule type="expression" dxfId="135" priority="6">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:XFD31">
-    <cfRule type="expression" dxfId="73" priority="5">
+    <cfRule type="expression" dxfId="134" priority="5">
       <formula>B$23="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="72" priority="4">
+    <cfRule type="expression" dxfId="133" priority="4">
       <formula>A$13="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21 A18:A19">
-    <cfRule type="expression" dxfId="71" priority="3">
+    <cfRule type="expression" dxfId="132" priority="3">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A31">
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="131" priority="2">
       <formula>A$13="LookUp"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A31">
-    <cfRule type="expression" dxfId="69" priority="1">
+    <cfRule type="expression" dxfId="130" priority="1">
       <formula>A$23="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49455,7 +49520,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="B32" sqref="B32"/>
@@ -49527,8 +49592,8 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="112" t="s">
+    <row r="11" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="113" t="s">
         <v>3021</v>
       </c>
     </row>
@@ -49558,11 +49623,11 @@
     </row>
     <row r="15" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>3518</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="112" t="s">
+        <v>3517</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="113" t="s">
         <v>3022</v>
       </c>
     </row>
@@ -49686,8 +49751,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="112" t="s">
+    <row r="29" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="113" t="s">
         <v>3023</v>
       </c>
     </row>
@@ -49834,8 +49899,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="112" t="s">
+    <row r="49" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="113" t="s">
         <v>3024</v>
       </c>
     </row>
@@ -49890,8 +49955,8 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="112" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="112" t="s">
+    <row r="55" spans="1:3" s="113" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="113" t="s">
         <v>3025</v>
       </c>
     </row>
@@ -49968,47 +50033,47 @@
     <mergeCell ref="A55:XFD55"/>
   </mergeCells>
   <conditionalFormatting sqref="B23:XFD23">
-    <cfRule type="expression" dxfId="68" priority="10">
+    <cfRule type="expression" dxfId="129" priority="10">
       <formula>B$22="Fixed Rate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:XFD26">
-    <cfRule type="expression" dxfId="67" priority="9">
+    <cfRule type="expression" dxfId="128" priority="9">
       <formula>AND(B$25&lt;&gt;"Auto Debit",B$25&lt;&gt;"Way Of Payment",B$25&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:XFD37 B31:C34 B37:C37">
-    <cfRule type="expression" dxfId="66" priority="8">
+    <cfRule type="expression" dxfId="127" priority="8">
       <formula>AND(B$30&lt;&gt;"",B$30&lt;&gt;"Copy Address From")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:XFD52">
-    <cfRule type="expression" dxfId="65" priority="7">
+    <cfRule type="expression" dxfId="126" priority="7">
       <formula>B$50="Lainnya"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:C36">
-    <cfRule type="expression" dxfId="64" priority="5">
+    <cfRule type="expression" dxfId="125" priority="5">
       <formula>AND(B$30&lt;&gt;"",B$30&lt;&gt;"Copy Address From")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="63" priority="4">
+    <cfRule type="expression" dxfId="124" priority="4">
       <formula>A$22="Fixed Rate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="62" priority="3">
+    <cfRule type="expression" dxfId="123" priority="3">
       <formula>AND(A$25&lt;&gt;"Auto Debit",A$25&lt;&gt;"Way Of Payment",A$25&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A37">
-    <cfRule type="expression" dxfId="61" priority="2">
+    <cfRule type="expression" dxfId="122" priority="2">
       <formula>AND(A$30&lt;&gt;"",A$30&lt;&gt;"Copy Address From")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:A52">
-    <cfRule type="expression" dxfId="60" priority="1">
+    <cfRule type="expression" dxfId="121" priority="1">
       <formula>A$50="Lainnya"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
flag failed verify ddl, lookup
</commit_message>
<xml_diff>
--- a/Excel/2.1 DataFile_NAP_CF4W.xlsx
+++ b/Excel/2.1 DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6630" tabRatio="769" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6630" tabRatio="769" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -15402,7 +15402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4928" uniqueCount="3570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4928" uniqueCount="3571">
   <si>
     <t>Count</t>
   </si>
@@ -26112,13 +26112,16 @@
     <t>checkstoreDB</t>
   </si>
   <si>
-    <t>0002APP20211204465</t>
-  </si>
-  <si>
     <t>WARNING</t>
   </si>
   <si>
     <t>Failed Delete[PT LOPO]</t>
+  </si>
+  <si>
+    <t>0002APP20211204472</t>
+  </si>
+  <si>
+    <t>06/27/2022</t>
   </si>
 </sst>
 </file>
@@ -29221,10 +29224,10 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection pane="topRight" activeCell="B33" sqref="B33"/>
+      <selection pane="topRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29656,9 +29659,9 @@
       <c r="A45" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="18" t="str">
+      <c r="B45" s="18" t="e">
         <f>VLOOKUP(B46,Master!$A:$B,2,FALSE)</f>
-        <v>EMP0006</v>
+        <v>#N/A</v>
       </c>
       <c r="C45" s="18" t="str">
         <f>VLOOKUP(C46,Master!$A:$B,2,FALSE)</f>
@@ -29668,9 +29671,6 @@
     <row r="46" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>107</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>329</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>329</v>
@@ -30147,11 +30147,11 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -30389,10 +30389,10 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31218,7 +31218,7 @@
       </c>
       <c r="B88" s="96">
         <f>IF(B24="Annualy",0,IF(B24="Full Tenor",ROUNDUP('6.TabApplicationData'!B20/12,0)-1,ROUNDUP(B28/12,0)-1))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -31233,7 +31233,7 @@
       </c>
       <c r="B90" s="96">
         <f>B88+1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -31422,7 +31422,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
@@ -31495,7 +31495,7 @@
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="116" customFormat="1" x14ac:dyDescent="0.25">
@@ -31722,7 +31722,7 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -31793,7 +31793,7 @@
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="116" customFormat="1" x14ac:dyDescent="0.25">
@@ -32508,7 +32508,7 @@
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
       <c r="C10" s="15"/>
     </row>
@@ -32674,7 +32674,7 @@
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -32684,19 +32684,19 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="D12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="E12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -33768,7 +33768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33834,7 +33834,7 @@
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!B10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="105" customFormat="1" x14ac:dyDescent="0.25">
@@ -33846,19 +33846,19 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="D12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="E12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -33989,9 +33989,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B45" sqref="B45"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34089,7 +34089,7 @@
         <v>3528</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>38</v>
+        <v>3532</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>50</v>
@@ -34125,8 +34125,8 @@
       <c r="A13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>3567</v>
+      <c r="B13" s="17" t="s">
+        <v>3569</v>
       </c>
       <c r="C13" t="s">
         <v>3564</v>
@@ -45823,7 +45823,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B58" sqref="B58"/>
     </sheetView>
@@ -46204,11 +46204,11 @@
       </c>
       <c r="B10" s="33" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
       <c r="C10" s="33" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
       <c r="D10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$D$10</f>
@@ -46248,11 +46248,11 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="D12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$D$13</f>
@@ -48420,7 +48420,7 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -48445,7 +48445,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -48462,7 +48462,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -48482,7 +48482,7 @@
         <v>3261</v>
       </c>
       <c r="B2" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -48535,7 +48535,7 @@
       </c>
       <c r="B10" s="33" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
       <c r="C10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$D$10</f>
@@ -48553,7 +48553,7 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$D$13</f>
@@ -49332,7 +49332,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C21" sqref="C21"/>
     </sheetView>
@@ -49423,7 +49423,7 @@
       </c>
       <c r="B10" s="33" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
       <c r="C10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$D$10</f>
@@ -49441,7 +49441,7 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$D$13</f>
@@ -49894,9 +49894,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49971,7 +49971,7 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -50198,11 +50198,11 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204465</v>
+        <v>0002APP20211204472</v>
       </c>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
@@ -50362,7 +50362,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
@@ -50439,7 +50439,7 @@
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$10</f>
-        <v>No</v>
+        <v>Edit</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="116" customFormat="1" x14ac:dyDescent="0.25">
@@ -50519,7 +50519,7 @@
         <v>3404</v>
       </c>
       <c r="B20" s="18">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C20" s="18">
         <v>37</v>
@@ -50530,7 +50530,7 @@
         <v>65</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -50568,7 +50568,7 @@
         <v>3407</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>224</v>
@@ -50655,7 +50655,7 @@
         <v>3373</v>
       </c>
       <c r="B34" s="18">
-        <v>40242</v>
+        <v>11530</v>
       </c>
       <c r="C34" s="18">
         <v>40242</v>
@@ -50666,7 +50666,7 @@
         <v>3374</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>3078</v>
+        <v>3256</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>3077</v>
@@ -50677,7 +50677,7 @@
         <v>3375</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>3077</v>
+        <v>3256</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>3078</v>
@@ -50688,7 +50688,7 @@
         <v>3410</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>3146</v>
+        <v>3257</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>3146</v>
@@ -50775,6 +50775,9 @@
       <c r="A51" s="18" t="s">
         <v>88</v>
       </c>
+      <c r="B51" s="18">
+        <v>111</v>
+      </c>
     </row>
     <row r="52" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="59" t="s">
@@ -50832,7 +50835,7 @@
         <v>93</v>
       </c>
       <c r="B57" s="18">
-        <v>1000</v>
+        <v>11</v>
       </c>
       <c r="C57" s="18">
         <v>1001</v>
@@ -50842,7 +50845,9 @@
       <c r="A58" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="34"/>
+      <c r="B58" s="34" t="s">
+        <v>3570</v>
+      </c>
       <c r="C58" s="34"/>
     </row>
     <row r="59" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
keyword insruance app view
</commit_message>
<xml_diff>
--- a/Excel/2.1 DataFile_NAP_CF4W.xlsx
+++ b/Excel/2.1 DataFile_NAP_CF4W.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-11END\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\git\NAP-CF4W-UF-NEW\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" tabRatio="769" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" tabRatio="769" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -25962,12 +25962,6 @@
     <t>TEST BUILDING OWNERSHIP</t>
   </si>
   <si>
-    <t>mama jodi</t>
-  </si>
-  <si>
-    <t>jodi@gmail.com</t>
-  </si>
-  <si>
     <t>JL KBN JRK</t>
   </si>
   <si>
@@ -26052,9 +26046,6 @@
     <t>1654897987213215</t>
   </si>
   <si>
-    <t>MOM CALVIN</t>
-  </si>
-  <si>
     <t>LookUp</t>
   </si>
   <si>
@@ -26115,43 +26106,52 @@
     <t>Failed Store DB</t>
   </si>
   <si>
+    <t>57943465avc</t>
+  </si>
+  <si>
+    <t>5646165dDa</t>
+  </si>
+  <si>
+    <t>654551rgsSd</t>
+  </si>
+  <si>
+    <t>abcg11ga2Ab</t>
+  </si>
+  <si>
+    <t>a2sB2gb321g</t>
+  </si>
+  <si>
+    <t>Age For This Customer Is Too Old ( &gt; 65 years)</t>
+  </si>
+  <si>
+    <t>Supplier Rate</t>
+  </si>
+  <si>
+    <t>mama Kennedy</t>
+  </si>
+  <si>
+    <t>12/02/2000</t>
+  </si>
+  <si>
+    <t>2839482738472837</t>
+  </si>
+  <si>
+    <t>DIMAS</t>
+  </si>
+  <si>
+    <t>mama dimas</t>
+  </si>
+  <si>
+    <t>dimas@gmail.com</t>
+  </si>
+  <si>
+    <t>0002APP20211205062</t>
+  </si>
+  <si>
+    <t>Validasi field invalid</t>
+  </si>
+  <si>
     <t>Gagal mendapatkan lookup</t>
-  </si>
-  <si>
-    <t>57943465avc</t>
-  </si>
-  <si>
-    <t>5646165dDa</t>
-  </si>
-  <si>
-    <t>654551rgsSd</t>
-  </si>
-  <si>
-    <t>abcg11ga2Ab</t>
-  </si>
-  <si>
-    <t>a2sB2gb321g</t>
-  </si>
-  <si>
-    <t>05/15/1991</t>
-  </si>
-  <si>
-    <t>Please Input Spouse Data in Family!</t>
-  </si>
-  <si>
-    <t>Customer age must be between 14 and 70 year old</t>
-  </si>
-  <si>
-    <t>Please do duplicate checking (MARIA JANE).</t>
-  </si>
-  <si>
-    <t>0002APP20211205052</t>
-  </si>
-  <si>
-    <t>Age For This Customer Is Too Old ( &gt; 65 years)</t>
-  </si>
-  <si>
-    <t>Supplier Rate</t>
   </si>
 </sst>
 </file>
@@ -29196,15 +29196,15 @@
       </c>
       <c r="B2" s="18">
         <f>COUNTA('2.TabFamilyData'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="18">
         <f>COUNTA('3a.TabGuarantorDataPersonal'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="18">
         <f>COUNTA('3b.TabGuarantorDataCompany'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <f>COUNTA('5.TabReferantorData'!$B$12:$XFD$12)</f>
@@ -29224,21 +29224,21 @@
         <v>3495</v>
       </c>
       <c r="B4" t="s">
-        <v>3531</v>
+        <v>3529</v>
       </c>
       <c r="C4" t="s">
-        <v>3532</v>
+        <v>3530</v>
       </c>
       <c r="D4" t="s">
-        <v>3535</v>
+        <v>3533</v>
       </c>
       <c r="E4" t="s">
-        <v>3539</v>
+        <v>3537</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>3541</v>
+        <v>3539</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
@@ -29268,10 +29268,10 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection pane="topRight" activeCell="C31" sqref="C31"/>
+      <selection pane="topRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29286,7 +29286,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3566</v>
+        <v>3563</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -29303,7 +29303,7 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3567</v>
+        <v>3564</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -29339,7 +29339,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -29568,7 +29568,7 @@
         <v>3418</v>
       </c>
       <c r="B29" s="116" t="s">
-        <v>3569</v>
+        <v>3565</v>
       </c>
       <c r="C29" s="81"/>
     </row>
@@ -29577,7 +29577,7 @@
         <v>3419</v>
       </c>
       <c r="B30" s="116" t="s">
-        <v>3570</v>
+        <v>3566</v>
       </c>
       <c r="C30" s="81"/>
     </row>
@@ -29586,7 +29586,7 @@
         <v>3420</v>
       </c>
       <c r="B31" s="116" t="s">
-        <v>3571</v>
+        <v>3567</v>
       </c>
       <c r="C31" s="81"/>
     </row>
@@ -29595,7 +29595,7 @@
         <v>3421</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>3572</v>
+        <v>3568</v>
       </c>
       <c r="C32" s="81"/>
     </row>
@@ -29604,7 +29604,7 @@
         <v>3422</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>3573</v>
+        <v>3569</v>
       </c>
       <c r="C33" s="7"/>
     </row>
@@ -30453,7 +30453,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="C88" sqref="C88"/>
@@ -30472,7 +30472,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3566</v>
+        <v>3563</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -30489,7 +30489,7 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3567</v>
+        <v>3564</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -30521,7 +30521,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -31203,7 +31203,7 @@
         <v>3189</v>
       </c>
       <c r="B82" t="s">
-        <v>3534</v>
+        <v>3532</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>3288</v>
@@ -31447,7 +31447,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C18" sqref="C18"/>
     </sheetView>
@@ -31483,7 +31483,7 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3579</v>
+        <v>3570</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -31515,7 +31515,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -31751,8 +31751,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31768,7 +31768,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3566</v>
+        <v>3563</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -31785,7 +31785,7 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3567</v>
+        <v>3564</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -31817,7 +31817,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -31883,7 +31883,7 @@
         <v>3474</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>3557</v>
+        <v>3554</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>3011</v>
@@ -32236,7 +32236,7 @@
     </row>
     <row r="50" spans="1:3" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>3580</v>
+        <v>3571</v>
       </c>
       <c r="B50" s="118"/>
       <c r="C50" s="118"/>
@@ -32534,7 +32534,7 @@
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
       <c r="C9" s="15"/>
     </row>
@@ -32705,7 +32705,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -32732,10 +32732,10 @@
         <v>3479</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>3538</v>
+        <v>3536</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>175</v>
@@ -32885,7 +32885,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -33390,7 +33390,7 @@
         <v>3387</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>3558</v>
+        <v>3555</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>3320</v>
@@ -33667,7 +33667,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -33870,12 +33870,12 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>3537</v>
+        <v>3535</v>
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!B10</f>
@@ -33899,7 +33899,7 @@
         <v>3481</v>
       </c>
       <c r="B13" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>3247</v>
@@ -33933,7 +33933,7 @@
         <v>3483</v>
       </c>
       <c r="B15" t="s">
-        <v>3555</v>
+        <v>3552</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>3248</v>
@@ -33967,7 +33967,7 @@
         <v>3484</v>
       </c>
       <c r="B17" t="s">
-        <v>3554</v>
+        <v>3551</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>3249</v>
@@ -34022,9 +34022,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B28" sqref="B28"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34038,7 +34038,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3566</v>
+        <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>8</v>
@@ -34057,8 +34057,8 @@
       <c r="A2" s="18" t="s">
         <v>3250</v>
       </c>
-      <c r="B2" t="s">
-        <v>3567</v>
+      <c r="B2" s="18" t="s">
+        <v>3053</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -34110,7 +34110,7 @@
     <row r="7" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -34119,7 +34119,7 @@
       </c>
       <c r="B9" s="115"/>
       <c r="C9" s="115" t="s">
-        <v>3526</v>
+        <v>3524</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -34161,10 +34161,10 @@
         <v>3578</v>
       </c>
       <c r="C13" t="s">
-        <v>3530</v>
+        <v>3528</v>
       </c>
       <c r="D13" t="s">
-        <v>3527</v>
+        <v>3525</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -34197,7 +34197,7 @@
         <v>3345</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3559</v>
+        <v>3556</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3011</v>
@@ -34217,7 +34217,7 @@
         <v>3346</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>6</v>
@@ -34237,7 +34237,7 @@
         <v>3347</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3546</v>
+        <v>3544</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3011</v>
@@ -34256,8 +34256,8 @@
       <c r="A19" s="59" t="s">
         <v>3348</v>
       </c>
-      <c r="B19" t="s">
-        <v>3545</v>
+      <c r="B19" s="18" t="s">
+        <v>3206</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>3206</v>
@@ -34297,7 +34297,7 @@
         <v>3350</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>346</v>
@@ -34316,9 +34316,7 @@
       <c r="A22" s="18" t="s">
         <v>2414</v>
       </c>
-      <c r="B22" s="72">
-        <v>45923</v>
-      </c>
+      <c r="B22" s="72"/>
       <c r="C22" s="72">
         <v>45924</v>
       </c>
@@ -34337,7 +34335,7 @@
         <v>3351</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>17</v>
@@ -34357,7 +34355,7 @@
         <v>3352</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3540</v>
+        <v>3538</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3203</v>
@@ -34417,7 +34415,7 @@
         <v>3355</v>
       </c>
       <c r="B27" s="117" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>3252</v>
@@ -34436,8 +34434,8 @@
       <c r="A28" s="59" t="s">
         <v>3356</v>
       </c>
-      <c r="B28" t="s">
-        <v>3546</v>
+      <c r="B28" s="4" t="s">
+        <v>3574</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3207</v>
@@ -34462,7 +34460,7 @@
         <v>3357</v>
       </c>
       <c r="B30" t="s">
-        <v>3547</v>
+        <v>3572</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>3208</v>
@@ -34781,7 +34779,7 @@
       <formula>A$14="Input Data"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31 G26:XFD31 A19:XFD24 A38:XFD45 A26:F30">
+  <conditionalFormatting sqref="A31 G26:XFD31 A38:XFD45 A26:F30 A19:XFD24">
     <cfRule type="expression" dxfId="155" priority="2">
       <formula>A$14="LookUp"</formula>
     </cfRule>
@@ -45855,9 +45853,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C49" sqref="C49"/>
+      <selection pane="topRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45875,10 +45873,10 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="17" t="s">
@@ -46178,10 +46176,10 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3576</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>3053</v>
+        <v>3579</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3580</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3053</v>
@@ -46229,7 +46227,7 @@
     <row r="8" spans="1:101" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:101" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:101" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -46284,6 +46282,10 @@
         <f>'1.TabCustomerMainData'!$B$13</f>
         <v>0002APP20211204995</v>
       </c>
+      <c r="C12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$B$13</f>
+        <v>0002APP20211205061</v>
+      </c>
     </row>
     <row r="13" spans="1:101" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
@@ -46293,7 +46295,7 @@
         <v>2416</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>3548</v>
+        <v>3545</v>
       </c>
       <c r="D13" s="48" t="s">
         <v>2416</v>
@@ -46315,10 +46317,10 @@
         <v>3345</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>3560</v>
+        <v>3557</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>3550</v>
+        <v>3547</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -46349,10 +46351,10 @@
         <v>3346</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>3555</v>
+        <v>3552</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>3549</v>
+        <v>3546</v>
       </c>
       <c r="D16" s="50" t="s">
         <v>3149</v>
@@ -46389,10 +46391,10 @@
         <v>3347</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>3561</v>
+        <v>3558</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>3553</v>
+        <v>3550</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
@@ -46423,7 +46425,7 @@
         <v>3369</v>
       </c>
       <c r="B18" s="47" t="s">
-        <v>380</v>
+        <v>9</v>
       </c>
       <c r="C18" s="47" t="s">
         <v>357</v>
@@ -46443,13 +46445,13 @@
         <v>3370</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>3555</v>
+        <v>3575</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>3549</v>
+        <v>3546</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>3523</v>
+        <v>3521</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>3210</v>
@@ -46636,7 +46638,7 @@
         <v>3351</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>210</v>
@@ -47001,13 +47003,13 @@
         <v>3356</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3542</v>
+        <v>3540</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>3525</v>
+        <v>3523</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>3212</v>
@@ -47126,7 +47128,7 @@
         <v>3357</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>3517</v>
+        <v>3576</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>3213</v>
@@ -47146,7 +47148,7 @@
         <v>3358</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>3518</v>
+        <v>3577</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>3214</v>
@@ -47673,7 +47675,7 @@
         <v>3359</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>3520</v>
+        <v>3518</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>39</v>
@@ -48303,7 +48305,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48319,10 +48321,10 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="18" t="s">
@@ -48336,8 +48338,8 @@
       <c r="A2" s="18" t="s">
         <v>3250</v>
       </c>
-      <c r="B2" t="s">
-        <v>3575</v>
+      <c r="B2" s="18" t="s">
+        <v>3053</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -48477,9 +48479,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48496,10 +48498,10 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" t="s">
+        <v>3563</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="18" t="s">
@@ -48513,11 +48515,11 @@
       <c r="A2" s="18" t="s">
         <v>3250</v>
       </c>
-      <c r="B2" t="s">
-        <v>3568</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="18" t="s">
         <v>3053</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3564</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3053</v>
@@ -48562,7 +48564,7 @@
     <row r="8" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -48591,14 +48593,17 @@
         <f>'1.TabCustomerMainData'!$B$13</f>
         <v>0002APP20211204995</v>
       </c>
-      <c r="C12" s="52"/>
+      <c r="C12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$B$13</f>
+        <v>0002APP20211205061</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>2415</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>3548</v>
+        <v>3545</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>2416</v>
@@ -48623,7 +48628,7 @@
         <v>3345</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3564</v>
+        <v>3561</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -48647,7 +48652,7 @@
         <v>3347</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3565</v>
+        <v>3562</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -48682,7 +48687,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>3521</v>
+        <v>3519</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3215</v>
@@ -48857,10 +48862,10 @@
         <v>3356</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3543</v>
+        <v>3541</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>3522</v>
+        <v>3520</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>3216</v>
@@ -49047,7 +49052,7 @@
         <v>3359</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>3551</v>
+        <v>3548</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>3072</v>
@@ -49372,9 +49377,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49390,10 +49395,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3566</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>8</v>
+        <v>3563</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3563</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>8</v>
@@ -49410,10 +49415,10 @@
         <v>3250</v>
       </c>
       <c r="B2" t="s">
-        <v>3567</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>3053</v>
+        <v>3580</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3564</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3053</v>
@@ -49461,7 +49466,7 @@
     <row r="8" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -49488,16 +49493,19 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211204995</v>
-      </c>
-      <c r="C12" s="52"/>
+        <v>0002APP20211205061</v>
+      </c>
+      <c r="C12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$B$13</f>
+        <v>0002APP20211205061</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>2415</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>3548</v>
+        <v>3545</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>2416</v>
@@ -49522,7 +49530,7 @@
         <v>3345</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>3563</v>
+        <v>3560</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -49534,7 +49542,7 @@
         <v>3346</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>3562</v>
+        <v>3559</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -49566,10 +49574,10 @@
         <v>3380</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>3562</v>
+        <v>3559</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>3528</v>
+        <v>3526</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3220</v>
@@ -49586,10 +49594,10 @@
         <v>3383</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3544</v>
+        <v>3542</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3529</v>
+        <v>3527</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>3221</v>
@@ -49671,7 +49679,7 @@
         <v>3359</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>3519</v>
+        <v>3517</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>3073</v>
@@ -49944,7 +49952,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49958,10 +49966,10 @@
       <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="18" t="s">
@@ -49975,8 +49983,8 @@
       <c r="A2" s="18" t="s">
         <v>3250</v>
       </c>
-      <c r="B2" t="s">
-        <v>3577</v>
+      <c r="B2" s="18" t="s">
+        <v>3053</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3053</v>
@@ -50027,7 +50035,7 @@
         <v>3346</v>
       </c>
       <c r="B13" t="s">
-        <v>3545</v>
+        <v>3543</v>
       </c>
       <c r="C13" s="86"/>
     </row>
@@ -50054,7 +50062,7 @@
         <v>3435</v>
       </c>
       <c r="B16" s="86" t="s">
-        <v>3555</v>
+        <v>3552</v>
       </c>
       <c r="C16" s="86"/>
     </row>
@@ -50079,7 +50087,7 @@
         <v>3437</v>
       </c>
       <c r="B19" s="114" t="s">
-        <v>3554</v>
+        <v>3551</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -50087,7 +50095,7 @@
         <v>3438</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>3552</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -50235,7 +50243,7 @@
     <row r="8" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -50243,7 +50251,7 @@
         <v>3509</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>3556</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="105" customFormat="1" x14ac:dyDescent="0.25">
@@ -50424,10 +50432,10 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50496,7 +50504,7 @@
     <row r="8" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3536</v>
+        <v>3534</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -50915,7 +50923,7 @@
         <v>94</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>3533</v>
+        <v>3531</v>
       </c>
       <c r="C58" s="34"/>
     </row>

</xml_diff>

<commit_message>
AITATR3-265 Revisi financial nap4
</commit_message>
<xml_diff>
--- a/Excel/2.1 DataFile_NAP_CF4W.xlsx
+++ b/Excel/2.1 DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="1" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" r:id="rId1" sheetId="5"/>
@@ -15532,7 +15532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5020" uniqueCount="3615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5000" uniqueCount="3620">
   <si>
     <t>Count</t>
   </si>
@@ -26098,9 +26098,6 @@
     <t>tono</t>
   </si>
   <si>
-    <t>128476912484214</t>
-  </si>
-  <si>
     <t>jono</t>
   </si>
   <si>
@@ -26110,21 +26107,9 @@
     <t>1274621476912448</t>
   </si>
   <si>
-    <t>0002APP20211204023</t>
-  </si>
-  <si>
     <t>0002APP20211204336</t>
   </si>
   <si>
-    <t>PT POLO</t>
-  </si>
-  <si>
-    <t>728374827384728</t>
-  </si>
-  <si>
-    <t>0002APP20211204347</t>
-  </si>
-  <si>
     <t>checksortpaging</t>
   </si>
   <si>
@@ -26167,15 +26152,6 @@
     <t>213817598636400</t>
   </si>
   <si>
-    <t>CALVIN CEN</t>
-  </si>
-  <si>
-    <t>1654897987213215</t>
-  </si>
-  <si>
-    <t>MOM CALVIN</t>
-  </si>
-  <si>
     <t>LookUp</t>
   </si>
   <si>
@@ -26191,12 +26167,6 @@
     <t>2183122030203339</t>
   </si>
   <si>
-    <t>FT TIO;FT COMPANY</t>
-  </si>
-  <si>
-    <t>MARIA JANE</t>
-  </si>
-  <si>
     <t>Edit</t>
   </si>
   <si>
@@ -26236,9 +26206,6 @@
     <t>Total Calculation DP Amount</t>
   </si>
   <si>
-    <t>214jnjo</t>
-  </si>
-  <si>
     <t>Total Fee</t>
   </si>
   <si>
@@ -26320,70 +26287,118 @@
     <t>ASASSSA</t>
   </si>
   <si>
-    <t>oksnd2382da</t>
-  </si>
-  <si>
-    <t>kisi23183ds</t>
-  </si>
-  <si>
-    <t>ksf2139db</t>
-  </si>
-  <si>
-    <t>skdn234dc</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
-    <t>05/15/1998</t>
-  </si>
-  <si>
     <t>U0005</t>
   </si>
   <si>
     <t>MRA_BLACKBOX</t>
   </si>
   <si>
+    <t>Cross Application / Agreement Information</t>
+  </si>
+  <si>
+    <t>Agreement No</t>
+  </si>
+  <si>
+    <t>Application No</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>0004AGR20211103603;0002AGR20211206782</t>
+  </si>
+  <si>
+    <t>0004APP20211100002;0002APP20211205472</t>
+  </si>
+  <si>
+    <t>MRA LIANA;SY FATUI</t>
+  </si>
+  <si>
+    <t>Edit NAP Back to Step</t>
+  </si>
+  <si>
+    <t>Budi</t>
+  </si>
+  <si>
+    <t>128476912484291</t>
+  </si>
+  <si>
+    <t>mama budi</t>
+  </si>
+  <si>
+    <t>budi@gmail.com</t>
+  </si>
+  <si>
+    <t>PT ASECA</t>
+  </si>
+  <si>
+    <t>728374827384153</t>
+  </si>
+  <si>
+    <t>FT LUIS;FT SANDI</t>
+  </si>
+  <si>
+    <t>TONO;PT LOPO</t>
+  </si>
+  <si>
+    <t>oksnd2382ED</t>
+  </si>
+  <si>
+    <t>kisi23182412</t>
+  </si>
+  <si>
+    <t>ksf2131235D</t>
+  </si>
+  <si>
+    <t>skdn2512</t>
+  </si>
+  <si>
+    <t>214jnjo124</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>FT SANDI;FT LUIS</t>
+  </si>
+  <si>
+    <t>Select SimilarData;Select ApplicationInProcess</t>
+  </si>
+  <si>
+    <t>0002APP20211205000</t>
+  </si>
+  <si>
+    <t>Button Save Tidak Berfungsi</t>
+  </si>
+  <si>
+    <t>Failed Data Lookup Tidak Sesuai DB</t>
+  </si>
+  <si>
+    <t>0002APP20211205592</t>
+  </si>
+  <si>
+    <t>HARTONO RACHMAT;PT LOPO</t>
+  </si>
+  <si>
+    <t>02/15/2001</t>
+  </si>
+  <si>
+    <t>IBU FT TIO</t>
+  </si>
+  <si>
+    <t>Please click Calculate Insurance.</t>
+  </si>
+  <si>
     <t>11,134,500</t>
   </si>
   <si>
-    <t>14.681933</t>
-  </si>
-  <si>
-    <t>Cross Application / Agreement Information</t>
-  </si>
-  <si>
-    <t>Agreement No</t>
-  </si>
-  <si>
-    <t>Application No</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>0004AGR20211103603;0002AGR20211206782</t>
-  </si>
-  <si>
-    <t>0004APP20211100002;0002APP20211205472</t>
-  </si>
-  <si>
-    <t>MRA LIANA;SY FATUI</t>
-  </si>
-  <si>
-    <t>Failed Data Lookup Tidak Sesuai DB</t>
-  </si>
-  <si>
-    <t>Edit NAP Back to Step</t>
-  </si>
-  <si>
-    <t>0002APP20211205465</t>
-  </si>
-  <si>
-    <t>CUST</t>
-  </si>
-  <si>
-    <t>Button Save Tidak Berfungsi</t>
+    <t>14.682159</t>
+  </si>
+  <si>
+    <t>Failed Verify Match / Equal</t>
   </si>
 </sst>
 </file>
@@ -26893,7 +26908,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="43"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="44"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="171">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
@@ -27085,6 +27100,7 @@
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="10" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="43" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0"/>
@@ -29443,19 +29459,19 @@
       </c>
       <c r="B2" s="18">
         <f>COUNTA('2.TabFamilyData'!$B$12:$XFD$12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="18">
         <f>COUNTA('3a.TabGuarantorDataPersonal'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="18">
         <f>COUNTA('3b.TabGuarantorDataCompany'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <f>COUNTA('5.TabReferantorData'!$B$12:$XFD$12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
         <f>COUNTA('7a.Accessories'!$B$12:$XFD$12)</f>
@@ -29471,21 +29487,21 @@
         <v>3494</v>
       </c>
       <c r="B4" t="s">
-        <v>3528</v>
+        <v>3523</v>
       </c>
       <c r="C4" t="s">
-        <v>3529</v>
+        <v>3524</v>
       </c>
       <c r="D4" t="s">
-        <v>3532</v>
+        <v>3527</v>
       </c>
       <c r="E4" t="s">
-        <v>3536</v>
+        <v>3531</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>3538</v>
+        <v>3533</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -29515,10 +29531,10 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection activeCell="C66" pane="topRight" sqref="C66"/>
+      <selection activeCell="A34" pane="topRight" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29533,7 +29549,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3544</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -29553,7 +29569,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3052</v>
+        <v>3545</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -29595,12 +29611,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -29612,14 +29628,14 @@
         <v>No</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="137" t="s">
+    <row customFormat="1" r="11" s="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="138" t="s">
         <v>3024</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="139"/>
     </row>
     <row customFormat="1" r="12" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -29663,14 +29679,14 @@
         <v>3078</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="137" t="s">
+    <row customFormat="1" r="16" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="138" t="s">
         <v>3025</v>
       </c>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="139"/>
+      <c r="E16" s="139"/>
     </row>
     <row customFormat="1" r="17" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
@@ -29829,7 +29845,7 @@
         <v>3417</v>
       </c>
       <c r="B29" s="116" t="s">
-        <v>3593</v>
+        <v>3601</v>
       </c>
       <c r="C29" s="81"/>
     </row>
@@ -29838,7 +29854,7 @@
         <v>3418</v>
       </c>
       <c r="B30" s="116" t="s">
-        <v>3594</v>
+        <v>3602</v>
       </c>
       <c r="C30" s="81"/>
     </row>
@@ -29847,7 +29863,7 @@
         <v>3419</v>
       </c>
       <c r="B31" s="116" t="s">
-        <v>3595</v>
+        <v>3603</v>
       </c>
       <c r="C31" s="81"/>
     </row>
@@ -29856,7 +29872,7 @@
         <v>3420</v>
       </c>
       <c r="B32" s="116" t="s">
-        <v>3596</v>
+        <v>3604</v>
       </c>
       <c r="C32" s="81"/>
     </row>
@@ -29865,15 +29881,15 @@
         <v>3421</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>3565</v>
+        <v>3605</v>
       </c>
       <c r="C33" s="7"/>
     </row>
-    <row customFormat="1" r="34" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="137" t="s">
+    <row customFormat="1" r="34" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="138" t="s">
         <v>3026</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="139"/>
     </row>
     <row customFormat="1" r="35" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="58" t="s">
@@ -29886,11 +29902,11 @@
         <v>3273</v>
       </c>
     </row>
-    <row customFormat="1" r="36" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="137" t="s">
+    <row customFormat="1" r="36" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="138" t="s">
         <v>3027</v>
       </c>
-      <c r="B36" s="138"/>
+      <c r="B36" s="139"/>
     </row>
     <row customFormat="1" r="37" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -29925,11 +29941,11 @@
         <v>282</v>
       </c>
     </row>
-    <row customFormat="1" r="40" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="137" t="s">
+    <row customFormat="1" r="40" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="138" t="s">
         <v>3028</v>
       </c>
-      <c r="B40" s="138"/>
+      <c r="B40" s="139"/>
     </row>
     <row customFormat="1" r="41" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
@@ -30040,11 +30056,11 @@
         <v>1231413</v>
       </c>
     </row>
-    <row customFormat="1" r="51" s="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="137" t="s">
+    <row customFormat="1" r="51" s="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="138" t="s">
         <v>3405</v>
       </c>
-      <c r="B51" s="138"/>
+      <c r="B51" s="139"/>
     </row>
     <row customFormat="1" r="52" s="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
@@ -30145,11 +30161,11 @@
         <v>3144</v>
       </c>
     </row>
-    <row customFormat="1" r="61" s="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="137" t="s">
+    <row customFormat="1" r="61" s="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="138" t="s">
         <v>3083</v>
       </c>
-      <c r="B61" s="138"/>
+      <c r="B61" s="139"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="109" t="s">
@@ -30167,15 +30183,15 @@
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
     </row>
-    <row customFormat="1" r="63" s="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="137" t="s">
-        <v>3558</v>
-      </c>
-      <c r="B63" s="138"/>
+    <row customFormat="1" r="63" s="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="138" t="s">
+        <v>3548</v>
+      </c>
+      <c r="B63" s="139"/>
     </row>
     <row customFormat="1" r="64" s="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>3559</v>
+        <v>3549</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>50</v>
@@ -30183,7 +30199,7 @@
     </row>
     <row customFormat="1" r="65" s="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>3560</v>
+        <v>3550</v>
       </c>
     </row>
     <row customFormat="1" r="66" s="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -30193,21 +30209,21 @@
     </row>
     <row customFormat="1" r="67" s="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>3561</v>
+        <v>3551</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>3597</v>
-      </c>
-    </row>
-    <row customFormat="1" r="68" s="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="137" t="s">
-        <v>3573</v>
-      </c>
-      <c r="B68" s="138"/>
+        <v>3582</v>
+      </c>
+    </row>
+    <row customFormat="1" r="68" s="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="138" t="s">
+        <v>3562</v>
+      </c>
+      <c r="B68" s="139"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="120" t="s">
-        <v>3563</v>
+        <v>3553</v>
       </c>
       <c r="B69" s="121">
         <f>B28/B19*100</f>
@@ -30216,7 +30232,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="120" t="s">
-        <v>3564</v>
+        <v>3554</v>
       </c>
       <c r="B70" s="121">
         <f>B19*B27%</f>
@@ -30393,7 +30409,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="B3" pane="topRight" sqref="B3"/>
+      <selection activeCell="B25" pane="topRight" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30409,7 +30425,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -30505,11 +30521,11 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
       <c r="C12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$C$13</f>
-        <v>0002APP20211204347</v>
+        <v>0002APP20211205000</v>
       </c>
     </row>
     <row customFormat="1" r="13" s="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -30559,10 +30575,10 @@
         <v>3439</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>3600</v>
+        <v>3584</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>3592</v>
+        <v>3581</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -30704,16 +30720,19 @@
       <c r="A21" s="18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row customFormat="1" r="22" s="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="137" t="s">
-        <v>3573</v>
-      </c>
-      <c r="B22" s="138"/>
+      <c r="B21" s="18" t="s">
+        <v>3606</v>
+      </c>
+    </row>
+    <row customFormat="1" r="22" s="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="138" t="s">
+        <v>3562</v>
+      </c>
+      <c r="B22" s="139"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="120" t="s">
-        <v>3563</v>
+        <v>3553</v>
       </c>
       <c r="B23" s="121">
         <f>B20/B17*100</f>
@@ -30726,7 +30745,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="120" t="s">
-        <v>3564</v>
+        <v>3554</v>
       </c>
       <c r="B24" s="121">
         <f>B17*B19%</f>
@@ -30788,7 +30807,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection activeCell="C90" pane="topRight" sqref="C90"/>
@@ -30807,7 +30826,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -30827,7 +30846,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3052</v>
+        <v>3616</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -30865,12 +30884,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -30882,14 +30901,14 @@
         <v>No</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="148" t="s">
+    <row customFormat="1" r="11" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
         <v>3029</v>
       </c>
-      <c r="B11" s="149"/>
-      <c r="C11" s="149"/>
-      <c r="D11" s="149"/>
-      <c r="E11" s="150"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="151"/>
     </row>
     <row customFormat="1" r="12" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -30902,14 +30921,14 @@
         <v>112</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="151" t="s">
+    <row customFormat="1" r="13" s="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="152" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="152"/>
-      <c r="C13" s="152"/>
-      <c r="D13" s="152"/>
-      <c r="E13" s="153"/>
+      <c r="B13" s="153"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="154"/>
     </row>
     <row customFormat="1" r="14" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
@@ -30970,14 +30989,14 @@
         <v>115</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="151" t="s">
+    <row customFormat="1" r="21" s="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="152" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="152"/>
-      <c r="C21" s="152"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="153"/>
+      <c r="B21" s="153"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="154"/>
     </row>
     <row customFormat="1" r="22" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
@@ -31050,14 +31069,14 @@
         <v>17</v>
       </c>
     </row>
-    <row customFormat="1" r="29" s="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="148" t="s">
+    <row customFormat="1" r="29" s="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="149" t="s">
         <v>3030</v>
       </c>
-      <c r="B29" s="149"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="149"/>
-      <c r="E29" s="150"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="150"/>
+      <c r="E29" s="151"/>
     </row>
     <row customFormat="1" r="30" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="64" t="s">
@@ -31092,14 +31111,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row customFormat="1" r="33" s="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="155" t="s">
+    <row customFormat="1" r="33" s="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="156" t="s">
         <v>3031</v>
       </c>
-      <c r="B33" s="156"/>
-      <c r="C33" s="156"/>
-      <c r="D33" s="156"/>
-      <c r="E33" s="157"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="157"/>
+      <c r="D33" s="157"/>
+      <c r="E33" s="158"/>
     </row>
     <row customFormat="1" r="34" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="59" t="s">
@@ -31112,14 +31131,14 @@
         <v>125</v>
       </c>
     </row>
-    <row customFormat="1" r="35" s="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="151" t="s">
+    <row customFormat="1" r="35" s="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="152" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="152"/>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
+      <c r="B35" s="153"/>
+      <c r="C35" s="153"/>
+      <c r="D35" s="153"/>
+      <c r="E35" s="153"/>
     </row>
     <row customFormat="1" r="36" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="s">
@@ -31211,14 +31230,14 @@
       <c r="D43" s="101"/>
       <c r="E43" s="101"/>
     </row>
-    <row customFormat="1" r="44" s="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="159" t="s">
+    <row customFormat="1" r="44" s="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="160" t="s">
         <v>3192</v>
       </c>
-      <c r="B44" s="160"/>
-      <c r="C44" s="160"/>
-      <c r="D44" s="160"/>
-      <c r="E44" s="160"/>
+      <c r="B44" s="161"/>
+      <c r="C44" s="161"/>
+      <c r="D44" s="161"/>
+      <c r="E44" s="161"/>
     </row>
     <row customFormat="1" r="45" s="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="89" t="s">
@@ -31258,14 +31277,14 @@
         <v>3180</v>
       </c>
     </row>
-    <row customFormat="1" r="49" s="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="161" t="s">
+    <row customFormat="1" r="49" s="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="162" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="162"/>
-      <c r="C49" s="162"/>
-      <c r="D49" s="162"/>
-      <c r="E49" s="162"/>
+      <c r="B49" s="163"/>
+      <c r="C49" s="163"/>
+      <c r="D49" s="163"/>
+      <c r="E49" s="163"/>
     </row>
     <row customFormat="1" r="50" s="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="89" t="s">
@@ -31339,8 +31358,8 @@
         <v>3183</v>
       </c>
     </row>
-    <row customFormat="1" r="58" s="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="163" t="s">
+    <row customFormat="1" r="58" s="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="164" t="s">
         <v>3168</v>
       </c>
     </row>
@@ -31532,11 +31551,11 @@
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
     </row>
-    <row customFormat="1" r="80" s="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="146" t="s">
+    <row customFormat="1" r="80" s="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="147" t="s">
         <v>3032</v>
       </c>
-      <c r="B80" s="147"/>
+      <c r="B80" s="148"/>
     </row>
     <row customFormat="1" r="81" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
@@ -31554,7 +31573,7 @@
         <v>3188</v>
       </c>
       <c r="B82" t="s">
-        <v>3531</v>
+        <v>3526</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>3287</v>
@@ -31581,17 +31600,17 @@
         <v>11134500</v>
       </c>
     </row>
-    <row customFormat="1" r="86" s="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="137" t="s">
-        <v>3572</v>
-      </c>
-      <c r="B86" s="164" t="s">
-        <v>3601</v>
+    <row customFormat="1" r="86" s="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="138" t="s">
+        <v>3561</v>
+      </c>
+      <c r="B86" s="165" t="s">
+        <v>3617</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>3566</v>
+        <v>3555</v>
       </c>
       <c r="B87" s="119">
         <f>SUM(B31:B32)</f>
@@ -31600,7 +31619,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
-        <v>3567</v>
+        <v>3556</v>
       </c>
       <c r="B88" s="119">
         <f>'7.TabAssetData'!B19</f>
@@ -31609,19 +31628,19 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="38" t="s">
-        <v>3568</v>
+        <v>3557</v>
       </c>
       <c r="B89" s="119">
         <f>B88+SUMIFS('7a.Accessories'!17:17,'7a.Accessories'!12:12,B8,'7a.Accessories'!4:4,"0",'7a.Accessories'!1:1,"SUCCESS")</f>
-        <v>600000000</v>
+        <v>610000000</v>
       </c>
     </row>
     <row customFormat="1" r="90" s="17" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="142" t="s">
+      <c r="A91" s="143" t="s">
         <v>3177</v>
       </c>
-      <c r="B91" s="143"/>
+      <c r="B91" s="144"/>
     </row>
     <row ht="30" r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="95" t="s">
@@ -31633,10 +31652,10 @@
       </c>
     </row>
     <row customHeight="1" ht="30" r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="144" t="s">
+      <c r="A93" s="145" t="s">
         <v>3176</v>
       </c>
-      <c r="B93" s="145"/>
+      <c r="B93" s="146"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="88" t="s">
@@ -31648,14 +31667,14 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="141" t="s">
+      <c r="A95" s="142" t="s">
         <v>3196</v>
       </c>
-      <c r="B95" s="141"/>
+      <c r="B95" s="142"/>
     </row>
     <row customHeight="1" ht="45.75" r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="141"/>
-      <c r="B96" s="141"/>
+      <c r="A96" s="142"/>
+      <c r="B96" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -31835,7 +31854,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="D14" pane="topRight" sqref="D14"/>
     </sheetView>
@@ -31853,8 +31872,8 @@
       <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>8</v>
+      <c r="B1" t="s">
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -31912,12 +31931,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -31929,8 +31948,8 @@
         <v>No</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="129" t="s">
+    <row customFormat="1" r="11" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="130" t="s">
         <v>3033</v>
       </c>
     </row>
@@ -31983,8 +32002,8 @@
         <v>100</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="129" t="s">
+    <row customFormat="1" r="17" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="130" t="s">
         <v>3034</v>
       </c>
     </row>
@@ -32032,8 +32051,8 @@
         <v>2449</v>
       </c>
     </row>
-    <row customFormat="1" r="22" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+    <row customFormat="1" r="22" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="130" t="s">
         <v>3035</v>
       </c>
     </row>
@@ -32153,7 +32172,7 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -32170,7 +32189,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3544</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -32190,7 +32209,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3052</v>
+        <v>3619</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -32228,12 +32247,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -32241,17 +32260,17 @@
         <v>3508</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>3552</v>
-      </c>
-    </row>
-    <row customFormat="1" r="11" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="148" t="s">
+        <v>3542</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
         <v>3036</v>
       </c>
-      <c r="B11" s="149"/>
-      <c r="C11" s="149"/>
-      <c r="D11" s="149"/>
-      <c r="E11" s="150"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="150"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="151"/>
     </row>
     <row customFormat="1" r="12" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
@@ -32312,14 +32331,14 @@
         <v>0</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="148" t="s">
+    <row customFormat="1" r="19" s="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="149" t="s">
         <v>3037</v>
       </c>
-      <c r="B19" s="149"/>
-      <c r="C19" s="149"/>
-      <c r="D19" s="149"/>
-      <c r="E19" s="149"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
     </row>
     <row customFormat="1" r="20" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
@@ -32563,14 +32582,14 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="42" s="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="148" t="s">
+    <row customFormat="1" r="42" s="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="149" t="s">
         <v>3038</v>
       </c>
-      <c r="B42" s="149"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149"/>
+      <c r="B42" s="150"/>
+      <c r="C42" s="150"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="150"/>
     </row>
     <row customFormat="1" r="43" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -32588,7 +32607,7 @@
         <v>170</v>
       </c>
       <c r="B44" t="s">
-        <v>3602</v>
+        <v>3618</v>
       </c>
       <c r="C44" s="2">
         <v>8</v>
@@ -32651,7 +32670,7 @@
     </row>
     <row customFormat="1" ht="15.75" r="50" s="12" spans="1:3" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>3556</v>
+        <v>3546</v>
       </c>
       <c r="B50" s="117"/>
       <c r="C50" s="117"/>
@@ -32669,7 +32688,7 @@
     </row>
     <row customFormat="1" r="52" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>3574</v>
+        <v>3563</v>
       </c>
       <c r="B52" s="18">
         <v>1000</v>
@@ -32677,7 +32696,7 @@
     </row>
     <row customFormat="1" r="53" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>3582</v>
+        <v>3571</v>
       </c>
       <c r="B53">
         <v>300000</v>
@@ -32685,21 +32704,21 @@
     </row>
     <row customFormat="1" r="54" s="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="123" t="s">
-        <v>3575</v>
+        <v>3564</v>
       </c>
     </row>
     <row customFormat="1" r="55" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>3576</v>
+        <v>3565</v>
       </c>
       <c r="B55" s="125">
         <f>SUM(B56:B57)</f>
-        <v>600000000</v>
+        <v>610000000</v>
       </c>
     </row>
     <row customFormat="1" r="56" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>3567</v>
+        <v>3556</v>
       </c>
       <c r="B56" s="125">
         <f>'7.TabAssetData'!B19</f>
@@ -32708,16 +32727,16 @@
     </row>
     <row customFormat="1" r="57" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>3577</v>
+        <v>3566</v>
       </c>
       <c r="B57" s="125">
         <f>SUMIFS('7a.Accessories'!17:17,'7a.Accessories'!12:12,B8,'7a.Accessories'!4:4,"0",'7a.Accessories'!1:1,"SUCCESS")</f>
-        <v>0</v>
+        <v>10000000</v>
       </c>
     </row>
     <row customFormat="1" r="58" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>3566</v>
+        <v>3555</v>
       </c>
       <c r="B58" s="125">
         <f>SUM(B21:B25,B39)</f>
@@ -32726,7 +32745,7 @@
     </row>
     <row customFormat="1" r="59" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>3578</v>
+        <v>3567</v>
       </c>
       <c r="B59" s="125">
         <f>SUM(B27,B29,B31,B33,B35,B41)</f>
@@ -32735,7 +32754,7 @@
     </row>
     <row customFormat="1" r="60" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>3579</v>
+        <v>3568</v>
       </c>
       <c r="B60" s="125">
         <f>'8.TabInsuranceData'!B85</f>
@@ -32744,34 +32763,34 @@
     </row>
     <row customFormat="1" r="61" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>3580</v>
+        <v>3569</v>
       </c>
       <c r="B61" s="125">
         <f>SUMIFS('7a.Accessories'!24:24,'7a.Accessories'!12:12,B8,'7a.Accessories'!4:4,"0",'7a.Accessories'!1:1,"SUCCESS")+'7.TabAssetData'!B70</f>
-        <v>120000000</v>
+        <v>122500000</v>
       </c>
     </row>
     <row customFormat="1" r="62" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>3581</v>
+        <v>3570</v>
       </c>
       <c r="B62" s="125">
         <f>B61-B53</f>
-        <v>119700000</v>
+        <v>122200000</v>
       </c>
     </row>
     <row customFormat="1" r="63" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>3591</v>
+        <v>3580</v>
       </c>
       <c r="B63" s="126">
         <f>IF(B37= "OTR-DP",B39/(B55-B61)*100,IF(B37="OTR-DP + Ins Cptlz + Fee Cptlz(Excl. Provision)",B39*100/(B55-B61+B60+(B59-B41))))</f>
-        <v>0.45760121376179719</v>
+        <v>0.45072611977896393</v>
       </c>
     </row>
     <row customFormat="1" r="64" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>3583</v>
+        <v>3572</v>
       </c>
       <c r="B64" s="125">
         <f>IF(B37= "OTR-DP",(B55-B61)*B38/100,IF(B37="OTR-DP + Ins Cptlz + Fee Cptlz(Excl. Provision)",(B55-B61+B60+(B59-B41))*B38/100))</f>
@@ -32780,56 +32799,56 @@
     </row>
     <row customFormat="1" r="65" s="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="122" t="s">
-        <v>3584</v>
+        <v>3573</v>
       </c>
     </row>
     <row customFormat="1" r="66" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>3585</v>
+        <v>3574</v>
       </c>
       <c r="B66">
-        <v>140676435</v>
+        <v>140598437</v>
       </c>
     </row>
     <row customFormat="1" r="67" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>3586</v>
+        <v>3575</v>
       </c>
       <c r="B67">
-        <v>506660115</v>
+        <v>506626688</v>
       </c>
     </row>
     <row customFormat="1" r="68" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>3587</v>
+        <v>3576</v>
       </c>
       <c r="B68">
-        <v>62017000</v>
+        <v>62013000</v>
       </c>
     </row>
     <row customFormat="1" r="69" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>3588</v>
+        <v>3577</v>
       </c>
       <c r="B69">
-        <v>51492885.490000002</v>
+        <v>51490310.549999997</v>
       </c>
     </row>
     <row customFormat="1" r="70" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>3589</v>
+        <v>3578</v>
       </c>
       <c r="B70">
-        <v>558153000.49000001</v>
+        <v>558116998.54999995</v>
       </c>
       <c r="C70" s="124"/>
     </row>
     <row customFormat="1" r="71" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>3590</v>
+        <v>3579</v>
       </c>
       <c r="B71">
-        <v>15.93666706</v>
+        <v>15.926756749999999</v>
       </c>
     </row>
   </sheetData>
@@ -33051,7 +33070,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>8</v>
@@ -33120,13 +33139,13 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
       <c r="C8" s="15"/>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
       <c r="C9" s="15"/>
     </row>
@@ -33198,10 +33217,10 @@
       <c r="C19" s="16"/>
     </row>
     <row customFormat="1" customHeight="1" ht="101.25" r="20" s="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="165" t="s">
+      <c r="A20" s="166" t="s">
         <v>2451</v>
       </c>
-      <c r="B20" s="165"/>
+      <c r="B20" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -33303,7 +33322,7 @@
     <row customFormat="1" r="8" s="18" spans="1:6" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -33322,7 +33341,7 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" ht="60" r="13" s="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -33330,10 +33349,10 @@
         <v>3478</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>3535</v>
+        <v>3530</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>3535</v>
+        <v>3530</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>174</v>
@@ -33417,7 +33436,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A9" pane="topRight" sqref="A9"/>
     </sheetView>
@@ -33434,7 +33453,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -33492,12 +33511,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -33529,14 +33548,14 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="146" t="s">
+    <row customFormat="1" r="13" s="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="147" t="s">
         <v>2441</v>
       </c>
-      <c r="B13" s="147"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="147"/>
-      <c r="E13" s="166"/>
+      <c r="B13" s="148"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="167"/>
     </row>
     <row customFormat="1" r="14" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -33734,14 +33753,14 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="26" s="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="146" t="s">
+    <row customFormat="1" r="26" s="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="147" t="s">
         <v>2445</v>
       </c>
-      <c r="B26" s="147"/>
-      <c r="C26" s="147"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="166"/>
+      <c r="B26" s="148"/>
+      <c r="C26" s="148"/>
+      <c r="D26" s="148"/>
+      <c r="E26" s="167"/>
     </row>
     <row customFormat="1" r="27" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -33982,11 +34001,11 @@
         <v>3318</v>
       </c>
     </row>
-    <row customFormat="1" r="42" s="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="146" t="s">
+    <row customFormat="1" r="42" s="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="147" t="s">
         <v>2434</v>
       </c>
-      <c r="B42" s="147"/>
+      <c r="B42" s="148"/>
     </row>
     <row customFormat="1" r="43" s="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -34002,7 +34021,7 @@
         <v>3386</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>3553</v>
+        <v>3543</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>3319</v>
@@ -34127,10 +34146,10 @@
       <c r="B54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="168" t="s">
+      <c r="A55" s="169" t="s">
         <v>2438</v>
       </c>
-      <c r="B55" s="169"/>
+      <c r="B55" s="170"/>
     </row>
     <row ht="210" r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
@@ -34215,7 +34234,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="A8" pane="topRight" sqref="A8"/>
+      <selection activeCell="C17" pane="topRight" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34230,7 +34249,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -34288,12 +34307,12 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -34398,7 +34417,7 @@
     </row>
     <row ht="15.75" r="17" spans="1:2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="118" t="s">
-        <v>3562</v>
+        <v>3552</v>
       </c>
       <c r="B17" s="119">
         <f>B12+B13+B14+B15+B16</f>
@@ -34440,7 +34459,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="F7" pane="topRight" sqref="F7"/>
+      <selection activeCell="E9" pane="topRight" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34454,8 +34473,8 @@
       <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>8</v>
+      <c r="B1" t="s">
+        <v>3544</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -34474,8 +34493,8 @@
       <c r="A2" s="18" t="s">
         <v>3249</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>3052</v>
+      <c r="B2" t="s">
+        <v>3619</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -34510,12 +34529,12 @@
     <row customFormat="1" r="8" s="18" spans="1:6" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>3534</v>
+        <v>3529</v>
       </c>
       <c r="B10" s="18" t="str">
         <f>'1.TabCustomerMainData'!B10</f>
@@ -34531,7 +34550,7 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="13" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -34539,7 +34558,7 @@
         <v>3480</v>
       </c>
       <c r="B13" t="s">
-        <v>3542</v>
+        <v>6</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>3246</v>
@@ -34573,7 +34592,7 @@
         <v>3482</v>
       </c>
       <c r="B15" t="s">
-        <v>3551</v>
+        <v>3607</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>3247</v>
@@ -34607,7 +34626,7 @@
         <v>3483</v>
       </c>
       <c r="B17" t="s">
-        <v>3550</v>
+        <v>3613</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>3248</v>
@@ -34664,7 +34683,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="B4" pane="topRight" sqref="B4"/>
+      <selection activeCell="C7" pane="topRight" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34758,15 +34777,12 @@
     <row customFormat="1" r="6" s="18" spans="1:13" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="7" s="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>3611</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>3613</v>
+        <v>3592</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>3612</v>
@@ -34777,9 +34793,7 @@
         <v>3507</v>
       </c>
       <c r="B9" s="115"/>
-      <c r="C9" s="115" t="s">
-        <v>3523</v>
-      </c>
+      <c r="C9" s="115"/>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
@@ -34822,11 +34836,11 @@
       <c r="B13" t="s">
         <v>3612</v>
       </c>
-      <c r="C13" t="s">
-        <v>3527</v>
+      <c r="C13" s="128" t="s">
+        <v>3609</v>
       </c>
       <c r="D13" t="s">
-        <v>3524</v>
+        <v>3522</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="15" r="14" s="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -34834,7 +34848,7 @@
         <v>2414</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>3545</v>
+        <v>3537</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>2415</v>
@@ -34849,8 +34863,8 @@
         <v>2415</v>
       </c>
     </row>
-    <row customFormat="1" r="15" s="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="129" t="s">
+    <row customFormat="1" r="15" s="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="130" t="s">
         <v>3013</v>
       </c>
     </row>
@@ -34859,7 +34873,7 @@
         <v>3344</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3569</v>
+        <v>3558</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3010</v>
@@ -34899,7 +34913,7 @@
         <v>3346</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3571</v>
+        <v>3560</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3010</v>
@@ -34919,7 +34933,7 @@
         <v>3347</v>
       </c>
       <c r="B19" t="s">
-        <v>3542</v>
+        <v>6</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>3205</v>
@@ -35019,7 +35033,7 @@
         <v>3351</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3537</v>
+        <v>3532</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3202</v>
@@ -35079,7 +35093,7 @@
         <v>3354</v>
       </c>
       <c r="B27" t="s">
-        <v>3598</v>
+        <v>3614</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>3251</v>
@@ -35099,7 +35113,7 @@
         <v>3355</v>
       </c>
       <c r="B28" t="s">
-        <v>3543</v>
+        <v>3560</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3206</v>
@@ -35124,7 +35138,7 @@
         <v>3356</v>
       </c>
       <c r="B30" t="s">
-        <v>3544</v>
+        <v>3615</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>3207</v>
@@ -35159,8 +35173,8 @@
         <v>3208</v>
       </c>
     </row>
-    <row customFormat="1" r="32" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="129" t="s">
+    <row customFormat="1" r="32" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="130" t="s">
         <v>3014</v>
       </c>
     </row>
@@ -35242,8 +35256,8 @@
         <v>207</v>
       </c>
     </row>
-    <row customFormat="1" r="37" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="129" t="s">
+    <row customFormat="1" r="37" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="130" t="s">
         <v>3015</v>
       </c>
     </row>
@@ -46522,7 +46536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="C12" pane="topRight" sqref="C12"/>
+      <selection activeCell="D13" pane="topRight" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46553,10 +46567,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>3554</v>
+        <v>3544</v>
       </c>
       <c r="H1" s="127" t="s">
-        <v>3554</v>
+        <v>3544</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>8</v>
@@ -46843,7 +46857,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3614</v>
+        <v>3052</v>
       </c>
       <c r="C2" s="127" t="s">
         <v>3052</v>
@@ -46858,10 +46872,10 @@
         <v>3052</v>
       </c>
       <c r="G2" s="127" t="s">
-        <v>3555</v>
+        <v>3545</v>
       </c>
       <c r="H2" s="127" t="s">
-        <v>3555</v>
+        <v>3545</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="18" spans="1:101" x14ac:dyDescent="0.25">
@@ -46900,7 +46914,7 @@
     <row customFormat="1" r="8" s="18" spans="1:101" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:101" x14ac:dyDescent="0.25">
@@ -46953,11 +46967,15 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205465</v>
+        <v>0002APP20211205592</v>
+      </c>
+      <c r="E12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$C$13</f>
+        <v>0002APP20211205000</v>
       </c>
     </row>
     <row customFormat="1" r="13" s="48" spans="1:101" x14ac:dyDescent="0.25">
@@ -46968,7 +46986,7 @@
         <v>2415</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>3545</v>
+        <v>3537</v>
       </c>
       <c r="D13" s="48" t="s">
         <v>2415</v>
@@ -46991,7 +47009,7 @@
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="51" t="s">
-        <v>3547</v>
+        <v>3539</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -47023,7 +47041,7 @@
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50" t="s">
-        <v>3546</v>
+        <v>3538</v>
       </c>
       <c r="D16" s="50" t="s">
         <v>3148</v>
@@ -47061,7 +47079,7 @@
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="51" t="s">
-        <v>3549</v>
+        <v>3541</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
@@ -47112,13 +47130,13 @@
         <v>3369</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>3570</v>
+        <v>3559</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>3546</v>
+        <v>3538</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>3209</v>
@@ -47670,13 +47688,13 @@
         <v>3355</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3539</v>
+        <v>3534</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>3211</v>
@@ -48026,110 +48044,110 @@
         <v>277</v>
       </c>
     </row>
-    <row customFormat="1" r="40" s="133" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A40" s="130" t="s">
+    <row customFormat="1" r="40" s="134" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A40" s="131" t="s">
         <v>3014</v>
       </c>
-      <c r="B40" s="131"/>
-      <c r="C40" s="131"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131"/>
-      <c r="H40" s="131"/>
-      <c r="I40" s="131"/>
-      <c r="J40" s="131"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="131"/>
-      <c r="M40" s="131"/>
-      <c r="N40" s="131"/>
-      <c r="O40" s="131"/>
-      <c r="P40" s="131"/>
-      <c r="Q40" s="131"/>
-      <c r="R40" s="131"/>
-      <c r="S40" s="131"/>
-      <c r="T40" s="131"/>
-      <c r="U40" s="131"/>
-      <c r="V40" s="131"/>
-      <c r="W40" s="131"/>
-      <c r="X40" s="131"/>
-      <c r="Y40" s="131"/>
-      <c r="Z40" s="131"/>
-      <c r="AA40" s="131"/>
-      <c r="AB40" s="131"/>
-      <c r="AC40" s="131"/>
-      <c r="AD40" s="131"/>
-      <c r="AE40" s="131"/>
-      <c r="AF40" s="131"/>
-      <c r="AG40" s="131"/>
-      <c r="AH40" s="131"/>
-      <c r="AI40" s="131"/>
-      <c r="AJ40" s="131"/>
-      <c r="AK40" s="131"/>
-      <c r="AL40" s="131"/>
-      <c r="AM40" s="131"/>
-      <c r="AN40" s="131"/>
-      <c r="AO40" s="131"/>
-      <c r="AP40" s="131"/>
-      <c r="AQ40" s="131"/>
-      <c r="AR40" s="131"/>
-      <c r="AS40" s="131"/>
-      <c r="AT40" s="131"/>
-      <c r="AU40" s="131"/>
-      <c r="AV40" s="131"/>
-      <c r="AW40" s="131"/>
-      <c r="AX40" s="131"/>
-      <c r="AY40" s="131"/>
-      <c r="AZ40" s="131"/>
-      <c r="BA40" s="131"/>
-      <c r="BB40" s="131"/>
-      <c r="BC40" s="131"/>
-      <c r="BD40" s="131"/>
-      <c r="BE40" s="131"/>
-      <c r="BF40" s="131"/>
-      <c r="BG40" s="131"/>
-      <c r="BH40" s="131"/>
-      <c r="BI40" s="131"/>
-      <c r="BJ40" s="131"/>
-      <c r="BK40" s="131"/>
-      <c r="BL40" s="131"/>
-      <c r="BM40" s="131"/>
-      <c r="BN40" s="131"/>
-      <c r="BO40" s="131"/>
-      <c r="BP40" s="131"/>
-      <c r="BQ40" s="131"/>
-      <c r="BR40" s="131"/>
-      <c r="BS40" s="131"/>
-      <c r="BT40" s="131"/>
-      <c r="BU40" s="131"/>
-      <c r="BV40" s="131"/>
-      <c r="BW40" s="131"/>
-      <c r="BX40" s="131"/>
-      <c r="BY40" s="131"/>
-      <c r="BZ40" s="131"/>
-      <c r="CA40" s="131"/>
-      <c r="CB40" s="131"/>
-      <c r="CC40" s="131"/>
-      <c r="CD40" s="131"/>
-      <c r="CE40" s="131"/>
-      <c r="CF40" s="131"/>
-      <c r="CG40" s="131"/>
-      <c r="CH40" s="131"/>
-      <c r="CI40" s="131"/>
-      <c r="CJ40" s="131"/>
-      <c r="CK40" s="131"/>
-      <c r="CL40" s="131"/>
-      <c r="CM40" s="131"/>
-      <c r="CN40" s="131"/>
-      <c r="CO40" s="131"/>
-      <c r="CP40" s="131"/>
-      <c r="CQ40" s="131"/>
-      <c r="CR40" s="131"/>
-      <c r="CS40" s="131"/>
-      <c r="CT40" s="131"/>
-      <c r="CU40" s="131"/>
-      <c r="CV40" s="131"/>
-      <c r="CW40" s="132"/>
+      <c r="B40" s="132"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="132"/>
+      <c r="G40" s="132"/>
+      <c r="H40" s="132"/>
+      <c r="I40" s="132"/>
+      <c r="J40" s="132"/>
+      <c r="K40" s="132"/>
+      <c r="L40" s="132"/>
+      <c r="M40" s="132"/>
+      <c r="N40" s="132"/>
+      <c r="O40" s="132"/>
+      <c r="P40" s="132"/>
+      <c r="Q40" s="132"/>
+      <c r="R40" s="132"/>
+      <c r="S40" s="132"/>
+      <c r="T40" s="132"/>
+      <c r="U40" s="132"/>
+      <c r="V40" s="132"/>
+      <c r="W40" s="132"/>
+      <c r="X40" s="132"/>
+      <c r="Y40" s="132"/>
+      <c r="Z40" s="132"/>
+      <c r="AA40" s="132"/>
+      <c r="AB40" s="132"/>
+      <c r="AC40" s="132"/>
+      <c r="AD40" s="132"/>
+      <c r="AE40" s="132"/>
+      <c r="AF40" s="132"/>
+      <c r="AG40" s="132"/>
+      <c r="AH40" s="132"/>
+      <c r="AI40" s="132"/>
+      <c r="AJ40" s="132"/>
+      <c r="AK40" s="132"/>
+      <c r="AL40" s="132"/>
+      <c r="AM40" s="132"/>
+      <c r="AN40" s="132"/>
+      <c r="AO40" s="132"/>
+      <c r="AP40" s="132"/>
+      <c r="AQ40" s="132"/>
+      <c r="AR40" s="132"/>
+      <c r="AS40" s="132"/>
+      <c r="AT40" s="132"/>
+      <c r="AU40" s="132"/>
+      <c r="AV40" s="132"/>
+      <c r="AW40" s="132"/>
+      <c r="AX40" s="132"/>
+      <c r="AY40" s="132"/>
+      <c r="AZ40" s="132"/>
+      <c r="BA40" s="132"/>
+      <c r="BB40" s="132"/>
+      <c r="BC40" s="132"/>
+      <c r="BD40" s="132"/>
+      <c r="BE40" s="132"/>
+      <c r="BF40" s="132"/>
+      <c r="BG40" s="132"/>
+      <c r="BH40" s="132"/>
+      <c r="BI40" s="132"/>
+      <c r="BJ40" s="132"/>
+      <c r="BK40" s="132"/>
+      <c r="BL40" s="132"/>
+      <c r="BM40" s="132"/>
+      <c r="BN40" s="132"/>
+      <c r="BO40" s="132"/>
+      <c r="BP40" s="132"/>
+      <c r="BQ40" s="132"/>
+      <c r="BR40" s="132"/>
+      <c r="BS40" s="132"/>
+      <c r="BT40" s="132"/>
+      <c r="BU40" s="132"/>
+      <c r="BV40" s="132"/>
+      <c r="BW40" s="132"/>
+      <c r="BX40" s="132"/>
+      <c r="BY40" s="132"/>
+      <c r="BZ40" s="132"/>
+      <c r="CA40" s="132"/>
+      <c r="CB40" s="132"/>
+      <c r="CC40" s="132"/>
+      <c r="CD40" s="132"/>
+      <c r="CE40" s="132"/>
+      <c r="CF40" s="132"/>
+      <c r="CG40" s="132"/>
+      <c r="CH40" s="132"/>
+      <c r="CI40" s="132"/>
+      <c r="CJ40" s="132"/>
+      <c r="CK40" s="132"/>
+      <c r="CL40" s="132"/>
+      <c r="CM40" s="132"/>
+      <c r="CN40" s="132"/>
+      <c r="CO40" s="132"/>
+      <c r="CP40" s="132"/>
+      <c r="CQ40" s="132"/>
+      <c r="CR40" s="132"/>
+      <c r="CS40" s="132"/>
+      <c r="CT40" s="132"/>
+      <c r="CU40" s="132"/>
+      <c r="CV40" s="132"/>
+      <c r="CW40" s="133"/>
     </row>
     <row customFormat="1" r="41" s="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A41" s="61" t="s">
@@ -48212,110 +48230,110 @@
         <v>296</v>
       </c>
     </row>
-    <row customFormat="1" r="45" s="130" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A45" s="130" t="s">
+    <row customFormat="1" r="45" s="131" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A45" s="131" t="s">
         <v>3015</v>
       </c>
-      <c r="B45" s="131"/>
-      <c r="C45" s="131"/>
-      <c r="D45" s="131"/>
-      <c r="E45" s="131"/>
-      <c r="F45" s="131"/>
-      <c r="G45" s="131"/>
-      <c r="H45" s="131"/>
-      <c r="I45" s="131"/>
-      <c r="J45" s="131"/>
-      <c r="K45" s="131"/>
-      <c r="L45" s="131"/>
-      <c r="M45" s="131"/>
-      <c r="N45" s="131"/>
-      <c r="O45" s="131"/>
-      <c r="P45" s="131"/>
-      <c r="Q45" s="131"/>
-      <c r="R45" s="131"/>
-      <c r="S45" s="131"/>
-      <c r="T45" s="131"/>
-      <c r="U45" s="131"/>
-      <c r="V45" s="131"/>
-      <c r="W45" s="131"/>
-      <c r="X45" s="131"/>
-      <c r="Y45" s="131"/>
-      <c r="Z45" s="131"/>
-      <c r="AA45" s="131"/>
-      <c r="AB45" s="131"/>
-      <c r="AC45" s="131"/>
-      <c r="AD45" s="131"/>
-      <c r="AE45" s="131"/>
-      <c r="AF45" s="131"/>
-      <c r="AG45" s="131"/>
-      <c r="AH45" s="131"/>
-      <c r="AI45" s="131"/>
-      <c r="AJ45" s="131"/>
-      <c r="AK45" s="131"/>
-      <c r="AL45" s="131"/>
-      <c r="AM45" s="131"/>
-      <c r="AN45" s="131"/>
-      <c r="AO45" s="131"/>
-      <c r="AP45" s="131"/>
-      <c r="AQ45" s="131"/>
-      <c r="AR45" s="131"/>
-      <c r="AS45" s="131"/>
-      <c r="AT45" s="131"/>
-      <c r="AU45" s="131"/>
-      <c r="AV45" s="131"/>
-      <c r="AW45" s="131"/>
-      <c r="AX45" s="131"/>
-      <c r="AY45" s="131"/>
-      <c r="AZ45" s="131"/>
-      <c r="BA45" s="131"/>
-      <c r="BB45" s="131"/>
-      <c r="BC45" s="131"/>
-      <c r="BD45" s="131"/>
-      <c r="BE45" s="131"/>
-      <c r="BF45" s="131"/>
-      <c r="BG45" s="131"/>
-      <c r="BH45" s="131"/>
-      <c r="BI45" s="131"/>
-      <c r="BJ45" s="131"/>
-      <c r="BK45" s="131"/>
-      <c r="BL45" s="131"/>
-      <c r="BM45" s="131"/>
-      <c r="BN45" s="131"/>
-      <c r="BO45" s="131"/>
-      <c r="BP45" s="131"/>
-      <c r="BQ45" s="131"/>
-      <c r="BR45" s="131"/>
-      <c r="BS45" s="131"/>
-      <c r="BT45" s="131"/>
-      <c r="BU45" s="131"/>
-      <c r="BV45" s="131"/>
-      <c r="BW45" s="131"/>
-      <c r="BX45" s="131"/>
-      <c r="BY45" s="131"/>
-      <c r="BZ45" s="131"/>
-      <c r="CA45" s="131"/>
-      <c r="CB45" s="131"/>
-      <c r="CC45" s="131"/>
-      <c r="CD45" s="131"/>
-      <c r="CE45" s="131"/>
-      <c r="CF45" s="131"/>
-      <c r="CG45" s="131"/>
-      <c r="CH45" s="131"/>
-      <c r="CI45" s="131"/>
-      <c r="CJ45" s="131"/>
-      <c r="CK45" s="131"/>
-      <c r="CL45" s="131"/>
-      <c r="CM45" s="131"/>
-      <c r="CN45" s="131"/>
-      <c r="CO45" s="131"/>
-      <c r="CP45" s="131"/>
-      <c r="CQ45" s="131"/>
-      <c r="CR45" s="131"/>
-      <c r="CS45" s="131"/>
-      <c r="CT45" s="131"/>
-      <c r="CU45" s="131"/>
-      <c r="CV45" s="131"/>
-      <c r="CW45" s="131"/>
+      <c r="B45" s="132"/>
+      <c r="C45" s="132"/>
+      <c r="D45" s="132"/>
+      <c r="E45" s="132"/>
+      <c r="F45" s="132"/>
+      <c r="G45" s="132"/>
+      <c r="H45" s="132"/>
+      <c r="I45" s="132"/>
+      <c r="J45" s="132"/>
+      <c r="K45" s="132"/>
+      <c r="L45" s="132"/>
+      <c r="M45" s="132"/>
+      <c r="N45" s="132"/>
+      <c r="O45" s="132"/>
+      <c r="P45" s="132"/>
+      <c r="Q45" s="132"/>
+      <c r="R45" s="132"/>
+      <c r="S45" s="132"/>
+      <c r="T45" s="132"/>
+      <c r="U45" s="132"/>
+      <c r="V45" s="132"/>
+      <c r="W45" s="132"/>
+      <c r="X45" s="132"/>
+      <c r="Y45" s="132"/>
+      <c r="Z45" s="132"/>
+      <c r="AA45" s="132"/>
+      <c r="AB45" s="132"/>
+      <c r="AC45" s="132"/>
+      <c r="AD45" s="132"/>
+      <c r="AE45" s="132"/>
+      <c r="AF45" s="132"/>
+      <c r="AG45" s="132"/>
+      <c r="AH45" s="132"/>
+      <c r="AI45" s="132"/>
+      <c r="AJ45" s="132"/>
+      <c r="AK45" s="132"/>
+      <c r="AL45" s="132"/>
+      <c r="AM45" s="132"/>
+      <c r="AN45" s="132"/>
+      <c r="AO45" s="132"/>
+      <c r="AP45" s="132"/>
+      <c r="AQ45" s="132"/>
+      <c r="AR45" s="132"/>
+      <c r="AS45" s="132"/>
+      <c r="AT45" s="132"/>
+      <c r="AU45" s="132"/>
+      <c r="AV45" s="132"/>
+      <c r="AW45" s="132"/>
+      <c r="AX45" s="132"/>
+      <c r="AY45" s="132"/>
+      <c r="AZ45" s="132"/>
+      <c r="BA45" s="132"/>
+      <c r="BB45" s="132"/>
+      <c r="BC45" s="132"/>
+      <c r="BD45" s="132"/>
+      <c r="BE45" s="132"/>
+      <c r="BF45" s="132"/>
+      <c r="BG45" s="132"/>
+      <c r="BH45" s="132"/>
+      <c r="BI45" s="132"/>
+      <c r="BJ45" s="132"/>
+      <c r="BK45" s="132"/>
+      <c r="BL45" s="132"/>
+      <c r="BM45" s="132"/>
+      <c r="BN45" s="132"/>
+      <c r="BO45" s="132"/>
+      <c r="BP45" s="132"/>
+      <c r="BQ45" s="132"/>
+      <c r="BR45" s="132"/>
+      <c r="BS45" s="132"/>
+      <c r="BT45" s="132"/>
+      <c r="BU45" s="132"/>
+      <c r="BV45" s="132"/>
+      <c r="BW45" s="132"/>
+      <c r="BX45" s="132"/>
+      <c r="BY45" s="132"/>
+      <c r="BZ45" s="132"/>
+      <c r="CA45" s="132"/>
+      <c r="CB45" s="132"/>
+      <c r="CC45" s="132"/>
+      <c r="CD45" s="132"/>
+      <c r="CE45" s="132"/>
+      <c r="CF45" s="132"/>
+      <c r="CG45" s="132"/>
+      <c r="CH45" s="132"/>
+      <c r="CI45" s="132"/>
+      <c r="CJ45" s="132"/>
+      <c r="CK45" s="132"/>
+      <c r="CL45" s="132"/>
+      <c r="CM45" s="132"/>
+      <c r="CN45" s="132"/>
+      <c r="CO45" s="132"/>
+      <c r="CP45" s="132"/>
+      <c r="CQ45" s="132"/>
+      <c r="CR45" s="132"/>
+      <c r="CS45" s="132"/>
+      <c r="CT45" s="132"/>
+      <c r="CU45" s="132"/>
+      <c r="CV45" s="132"/>
+      <c r="CW45" s="132"/>
     </row>
     <row customFormat="1" r="46" s="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
@@ -48760,16 +48778,16 @@
       </c>
     </row>
     <row customHeight="1" ht="15" r="60" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A60" s="134" t="s">
+      <c r="A60" s="135" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="134" t="s">
+      <c r="B60" s="135" t="s">
         <v>3157</v>
       </c>
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A61" s="135"/>
-      <c r="B61" s="135"/>
+      <c r="A61" s="136"/>
+      <c r="B61" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -49099,17 +49117,17 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customHeight="1" ht="60" r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="136" t="s">
+      <c r="B14" s="137" t="s">
         <v>3158</v>
       </c>
-      <c r="C14" s="136"/>
+      <c r="C14" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -49124,9 +49142,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="A12" pane="topRight" sqref="A12"/>
+      <selection activeCell="B28" pane="topRight" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49160,7 +49178,7 @@
       <c r="A2" s="18" t="s">
         <v>3249</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="18" t="s">
         <v>3052</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -49212,7 +49230,7 @@
     <row customFormat="1" r="8" s="18" spans="1:6" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -49239,9 +49257,12 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
-      </c>
-      <c r="C12" s="52"/>
+        <v>0002APP20211205592</v>
+      </c>
+      <c r="C12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$C$13</f>
+        <v>0002APP20211205000</v>
+      </c>
     </row>
     <row customFormat="1" r="13" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
@@ -49263,8 +49284,8 @@
         <v>2415</v>
       </c>
     </row>
-    <row customFormat="1" r="14" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="129" t="s">
+    <row customFormat="1" r="14" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="130" t="s">
         <v>3018</v>
       </c>
     </row>
@@ -49306,7 +49327,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>9</v>
+        <v>237</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>9</v>
@@ -49326,7 +49347,7 @@
         <v>3518</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>3518</v>
+        <v>3593</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3214</v>
@@ -49501,10 +49522,10 @@
         <v>3355</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3540</v>
+        <v>3535</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>3519</v>
+        <v>3594</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>3215</v>
@@ -49534,7 +49555,7 @@
         <v>3217</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>3217</v>
+        <v>3595</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>3217</v>
@@ -49554,7 +49575,7 @@
         <v>3218</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>3218</v>
+        <v>3596</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>3218</v>
@@ -49566,8 +49587,8 @@
         <v>3218</v>
       </c>
     </row>
-    <row customFormat="1" r="32" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="129" t="s">
+    <row customFormat="1" r="32" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="130" t="s">
         <v>3014</v>
       </c>
     </row>
@@ -49661,8 +49682,8 @@
         <v>34</v>
       </c>
     </row>
-    <row customFormat="1" r="37" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="129" t="s">
+    <row customFormat="1" r="37" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="130" t="s">
         <v>3015</v>
       </c>
     </row>
@@ -49674,7 +49695,7 @@
         <v>50</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>38</v>
@@ -49690,9 +49711,6 @@
       <c r="A39" s="59" t="s">
         <v>3358</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>3071</v>
-      </c>
       <c r="D39" s="18" t="s">
         <v>3071</v>
       </c>
@@ -49708,9 +49726,7 @@
         <v>3359</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>3070</v>
-      </c>
+      <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>3070</v>
       </c>
@@ -49726,9 +49742,7 @@
         <v>3360</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>110</v>
       </c>
@@ -49744,9 +49758,7 @@
         <v>3361</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>42</v>
       </c>
@@ -49761,9 +49773,6 @@
       <c r="A43" s="59" t="s">
         <v>3362</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D43" s="18" t="s">
         <v>43</v>
       </c>
@@ -49778,9 +49787,6 @@
       <c r="A44" s="59" t="s">
         <v>3363</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D44" s="18" t="s">
         <v>43</v>
       </c>
@@ -49795,9 +49801,6 @@
       <c r="A45" s="59" t="s">
         <v>3364</v>
       </c>
-      <c r="C45" s="18" t="s">
-        <v>2416</v>
-      </c>
       <c r="D45" s="18" t="s">
         <v>2416</v>
       </c>
@@ -49811,9 +49814,6 @@
     <row customFormat="1" r="46" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="59" t="s">
         <v>3380</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>45</v>
@@ -49995,9 +49995,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="A12" pane="topRight" sqref="A12"/>
+      <selection activeCell="C7" pane="topRight" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50013,7 +50013,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3554</v>
+        <v>3544</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -50033,7 +50033,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3614</v>
+        <v>3610</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -50084,7 +50084,7 @@
     <row customFormat="1" r="8" s="18" spans="1:6" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -50111,9 +50111,12 @@
       </c>
       <c r="B12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
-      </c>
-      <c r="C12" s="52"/>
+        <v>0002APP20211205592</v>
+      </c>
+      <c r="C12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$C$13</f>
+        <v>0002APP20211205000</v>
+      </c>
     </row>
     <row customFormat="1" r="13" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
@@ -50135,8 +50138,8 @@
         <v>2415</v>
       </c>
     </row>
-    <row customFormat="1" r="14" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="129" t="s">
+    <row customFormat="1" r="14" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="130" t="s">
         <v>3018</v>
       </c>
     </row>
@@ -50185,10 +50188,10 @@
         <v>3379</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>3557</v>
+        <v>3547</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>3525</v>
+        <v>3597</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3219</v>
@@ -50205,10 +50208,10 @@
         <v>3382</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3541</v>
+        <v>3536</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3526</v>
+        <v>3598</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>3220</v>
@@ -50260,8 +50263,8 @@
         <v>55</v>
       </c>
     </row>
-    <row customFormat="1" r="22" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+    <row customFormat="1" r="22" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="130" t="s">
         <v>3015</v>
       </c>
     </row>
@@ -50273,7 +50276,7 @@
         <v>50</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>38</v>
@@ -50289,9 +50292,6 @@
       <c r="A24" s="59" t="s">
         <v>3358</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>3072</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3072</v>
       </c>
@@ -50307,9 +50307,7 @@
         <v>3359</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2">
-        <v>6</v>
-      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2">
         <v>6</v>
       </c>
@@ -50325,9 +50323,7 @@
         <v>3360</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2">
-        <v>2</v>
-      </c>
+      <c r="C26" s="2"/>
       <c r="D26" s="2">
         <v>2</v>
       </c>
@@ -50343,9 +50339,7 @@
         <v>3361</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>3267</v>
       </c>
@@ -50360,9 +50354,6 @@
       <c r="A28" s="59" t="s">
         <v>3362</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D28" s="18" t="s">
         <v>56</v>
       </c>
@@ -50377,9 +50368,6 @@
       <c r="A29" s="59" t="s">
         <v>3363</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D29" s="18" t="s">
         <v>56</v>
       </c>
@@ -50394,9 +50382,6 @@
       <c r="A30" s="59" t="s">
         <v>3364</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>2416</v>
-      </c>
       <c r="D30" s="18" t="s">
         <v>2416</v>
       </c>
@@ -50410,9 +50395,6 @@
     <row customFormat="1" r="31" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="59" t="s">
         <v>3380</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>44</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>44</v>
@@ -50542,7 +50524,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="A12" pane="topRight" sqref="A12"/>
+      <selection activeCell="C8" pane="topRight" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50557,7 +50539,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -50576,7 +50558,7 @@
       <c r="A2" s="18" t="s">
         <v>3249</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="18" t="s">
         <v>3052</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -50623,7 +50605,7 @@
       </c>
       <c r="B12" s="18" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
     </row>
     <row customFormat="1" r="13" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -50631,7 +50613,7 @@
         <v>3345</v>
       </c>
       <c r="B13" t="s">
-        <v>3542</v>
+        <v>6</v>
       </c>
       <c r="C13" s="86"/>
     </row>
@@ -50658,16 +50640,16 @@
         <v>3434</v>
       </c>
       <c r="B16" s="86" t="s">
-        <v>3551</v>
+        <v>3599</v>
       </c>
       <c r="C16" s="86"/>
     </row>
-    <row customFormat="1" r="17" s="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="17" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="85" t="s">
         <v>3435</v>
       </c>
       <c r="B17" s="86" t="s">
-        <v>3504</v>
+        <v>3540</v>
       </c>
       <c r="C17" s="114"/>
     </row>
@@ -50683,15 +50665,15 @@
         <v>3436</v>
       </c>
       <c r="B19" s="114" t="s">
-        <v>3550</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="30" r="20" s="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3600</v>
+      </c>
+    </row>
+    <row customFormat="1" r="20" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="85" t="s">
         <v>3437</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>3548</v>
+        <v>3608</v>
       </c>
     </row>
     <row customFormat="1" r="21" s="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -50730,7 +50712,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="C7" pane="topRight" sqref="C7"/>
+      <selection activeCell="C12" pane="topRight" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50750,8 +50732,8 @@
       <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>8</v>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>8</v>
@@ -50839,7 +50821,7 @@
     <row customFormat="1" r="8" s="18" spans="1:10" x14ac:dyDescent="0.25"/>
     <row customFormat="1" r="9" s="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -50847,7 +50829,10 @@
         <v>3508</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>3552</v>
+        <v>38</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row customFormat="1" r="11" s="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -50866,10 +50851,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="52" t="str">
+        <f>'1.TabCustomerMainData'!$C$13</f>
+        <v>0002APP20211205000</v>
+      </c>
+      <c r="C12" s="52" t="str">
         <f>'1.TabCustomerMainData'!$B$13</f>
-        <v>0002APP20211205496</v>
-      </c>
-      <c r="C12" s="52"/>
+        <v>0002APP20211205592</v>
+      </c>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
@@ -51013,7 +51001,7 @@
     <dataValidation allowBlank="1" errorStyle="information" showErrorMessage="1" showInputMessage="1" sqref="B17:J17" type="list">
       <formula1>"Gross, Nett"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B10:C10" type="list">
       <formula1>"Yes, No, Edit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -51028,10 +51016,10 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection activeCell="A62" pane="topRight" sqref="A62:XFD65"/>
+      <selection activeCell="B65" pane="topRight" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51047,7 +51035,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3554</v>
+        <v>3544</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>8</v>
@@ -51067,7 +51055,7 @@
         <v>3249</v>
       </c>
       <c r="B2" t="s">
-        <v>3610</v>
+        <v>3611</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3052</v>
@@ -51109,16 +51097,16 @@
       </c>
       <c r="B8" s="18" t="str">
         <f>'1.TabCustomerMainData'!B$13</f>
-        <v>0002APP20211205496</v>
+        <v>0002APP20211205592</v>
       </c>
       <c r="C8" s="18" t="str">
         <f>'1.TabCustomerMainData'!C$13</f>
-        <v>0002APP20211204347</v>
+        <v>0002APP20211205000</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>3533</v>
+        <v>3528</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -51130,8 +51118,8 @@
         <v>No</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="129" t="s">
+    <row customFormat="1" r="11" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="130" t="s">
         <v>3019</v>
       </c>
     </row>
@@ -51140,7 +51128,7 @@
         <v>3388</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>3599</v>
+        <v>3583</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3225</v>
@@ -51167,8 +51155,8 @@
         <v>3487</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="129" t="s">
+    <row customFormat="1" r="16" s="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="130" t="s">
         <v>3020</v>
       </c>
     </row>
@@ -51298,8 +51286,8 @@
         <v>72</v>
       </c>
     </row>
-    <row customFormat="1" r="29" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="129" t="s">
+    <row customFormat="1" r="29" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="130" t="s">
         <v>3021</v>
       </c>
     </row>
@@ -51449,8 +51437,8 @@
         <v>85</v>
       </c>
     </row>
-    <row customFormat="1" r="49" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="129" t="s">
+    <row customFormat="1" r="49" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="130" t="s">
         <v>3022</v>
       </c>
     </row>
@@ -51508,8 +51496,8 @@
         <v>2292</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="55" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="129" t="s">
+    <row customFormat="1" customHeight="1" ht="13.5" r="55" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="130" t="s">
         <v>3023</v>
       </c>
     </row>
@@ -51540,7 +51528,7 @@
         <v>93</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>3530</v>
+        <v>3525</v>
       </c>
       <c r="C58" s="34"/>
     </row>
@@ -51579,33 +51567,33 @@
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="14.25" r="62" s="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="129" t="s">
-        <v>3603</v>
+    <row customFormat="1" customHeight="1" ht="14.25" r="62" s="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="130" t="s">
+        <v>3585</v>
       </c>
     </row>
     <row customFormat="1" r="63" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>3605</v>
+        <v>3587</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>3608</v>
+        <v>3590</v>
       </c>
     </row>
     <row customFormat="1" r="64" s="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>3604</v>
+        <v>3586</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>3607</v>
+        <v>3589</v>
       </c>
     </row>
     <row customFormat="1" r="65" s="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>3606</v>
+        <v>3588</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>3609</v>
+        <v>3591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisi store db nap4 tab other attribute
</commit_message>
<xml_diff>
--- a/Excel/2.1 DataFile_NAP_CF4W.xlsx
+++ b/Excel/2.1 DataFile_NAP_CF4W.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-Sprint17\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\git\NAP-CF4W-UF-NEW\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="15" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -15584,7 +15584,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="3650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="3643">
   <si>
     <t>Count</t>
   </si>
@@ -26504,40 +26504,19 @@
     <t>ond2D1v3cx13</t>
   </si>
   <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>Failed Store DB</t>
-  </si>
-  <si>
-    <t>Button Save Tidak Berfungsi</t>
-  </si>
-  <si>
-    <t>Failed Verify Rule</t>
-  </si>
-  <si>
     <t>21871000</t>
   </si>
   <si>
     <t>0002APP20211205843</t>
   </si>
   <si>
-    <t>Failed Data Lookup Tidak Sesuai DB</t>
-  </si>
-  <si>
     <t>15000;6786500;0</t>
   </si>
   <si>
-    <t>WARNING</t>
-  </si>
-  <si>
     <t>14.692175</t>
   </si>
   <si>
     <t>0002APP20211205844</t>
-  </si>
-  <si>
-    <t>Double Financing with Application 0002APP20211205841</t>
   </si>
   <si>
     <t>DP Nett Percentage</t>
@@ -27304,6 +27283,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -27363,9 +27345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -29781,10 +29760,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -29804,10 +29783,10 @@
         <v>3210</v>
       </c>
       <c r="B2" t="s">
-        <v>3639</v>
+        <v>3046</v>
       </c>
       <c r="C2" t="s">
-        <v>3648</v>
+        <v>3046</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3046</v>
@@ -29872,14 +29851,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="164" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="161" t="s">
+    <row r="11" spans="1:7" s="167" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="164" t="s">
         <v>3018</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="162"/>
+      <c r="B11" s="165"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
     </row>
     <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -29925,14 +29904,14 @@
         <v>3071</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="161" t="s">
+    <row r="16" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="164" t="s">
         <v>3019</v>
       </c>
-      <c r="B16" s="162"/>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162"/>
-      <c r="E16" s="162"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
     </row>
     <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
@@ -30141,11 +30120,11 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="161" t="s">
+    <row r="34" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="164" t="s">
         <v>3020</v>
       </c>
-      <c r="B34" s="162"/>
+      <c r="B34" s="165"/>
     </row>
     <row r="35" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="58" t="s">
@@ -30158,11 +30137,11 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="161" t="s">
+    <row r="36" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="164" t="s">
         <v>3021</v>
       </c>
-      <c r="B36" s="162"/>
+      <c r="B36" s="165"/>
     </row>
     <row r="37" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -30197,11 +30176,11 @@
         <v>278</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="161" t="s">
+    <row r="40" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="164" t="s">
         <v>3022</v>
       </c>
-      <c r="B40" s="162"/>
+      <c r="B40" s="165"/>
     </row>
     <row r="41" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
@@ -30315,11 +30294,11 @@
         <v>1231413</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="161" t="s">
+    <row r="51" spans="1:8" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="164" t="s">
         <v>3332</v>
       </c>
-      <c r="B51" s="162"/>
+      <c r="B51" s="165"/>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
@@ -30420,11 +30399,11 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="161" t="s">
+    <row r="61" spans="1:8" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="164" t="s">
         <v>3076</v>
       </c>
-      <c r="B61" s="162"/>
+      <c r="B61" s="165"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="107" t="s">
@@ -30442,11 +30421,11 @@
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
     </row>
-    <row r="63" spans="1:8" s="163" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="161" t="s">
+    <row r="63" spans="1:8" s="166" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="164" t="s">
         <v>3455</v>
       </c>
-      <c r="B63" s="162"/>
+      <c r="B63" s="165"/>
     </row>
     <row r="64" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
@@ -30474,11 +30453,11 @@
         <v>3487</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="161" t="s">
+    <row r="68" spans="1:3" s="166" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="164" t="s">
         <v>3468</v>
       </c>
-      <c r="B68" s="162"/>
+      <c r="B68" s="165"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="117" t="s">
@@ -30694,10 +30673,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -30993,11 +30972,11 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="163" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="161" t="s">
+    <row r="22" spans="1:8" s="166" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="164" t="s">
         <v>3468</v>
       </c>
-      <c r="B22" s="162"/>
+      <c r="B22" s="165"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="117" t="s">
@@ -31095,10 +31074,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -31118,10 +31097,10 @@
         <v>3210</v>
       </c>
       <c r="B2" t="s">
-        <v>3638</v>
+        <v>3046</v>
       </c>
       <c r="C2" t="s">
-        <v>3638</v>
+        <v>3046</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3046</v>
@@ -31188,14 +31167,14 @@
         <v>No</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="170" t="s">
+    <row r="11" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="173" t="s">
         <v>3023</v>
       </c>
-      <c r="B11" s="171"/>
-      <c r="C11" s="171"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172"/>
+      <c r="B11" s="174"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
     </row>
     <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -31208,14 +31187,14 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="176" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="173" t="s">
+    <row r="13" spans="1:7" s="179" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="174"/>
-      <c r="C13" s="174"/>
-      <c r="D13" s="174"/>
-      <c r="E13" s="175"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="178"/>
     </row>
     <row r="14" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
@@ -31276,14 +31255,14 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="176" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="173" t="s">
+    <row r="21" spans="1:5" s="179" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="174"/>
-      <c r="C21" s="174"/>
-      <c r="D21" s="174"/>
-      <c r="E21" s="175"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="178"/>
     </row>
     <row r="22" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
@@ -31356,14 +31335,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="170" t="s">
+    <row r="29" spans="1:5" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="173" t="s">
         <v>3024</v>
       </c>
-      <c r="B29" s="171"/>
-      <c r="C29" s="171"/>
-      <c r="D29" s="171"/>
-      <c r="E29" s="172"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="175"/>
     </row>
     <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="64" t="s">
@@ -31398,14 +31377,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="180" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="177" t="s">
+    <row r="33" spans="1:5" s="183" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="180" t="s">
         <v>3025</v>
       </c>
-      <c r="B33" s="178"/>
-      <c r="C33" s="178"/>
-      <c r="D33" s="178"/>
-      <c r="E33" s="179"/>
+      <c r="B33" s="181"/>
+      <c r="C33" s="181"/>
+      <c r="D33" s="181"/>
+      <c r="E33" s="182"/>
     </row>
     <row r="34" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="59" t="s">
@@ -31517,14 +31496,14 @@
       <c r="D43" s="99"/>
       <c r="E43" s="99"/>
     </row>
-    <row r="44" spans="1:5" s="181" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="181" t="s">
+    <row r="44" spans="1:5" s="184" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="184" t="s">
         <v>3172</v>
       </c>
-      <c r="B44" s="182"/>
-      <c r="C44" s="182"/>
-      <c r="D44" s="182"/>
-      <c r="E44" s="182"/>
+      <c r="B44" s="185"/>
+      <c r="C44" s="185"/>
+      <c r="D44" s="185"/>
+      <c r="E44" s="185"/>
     </row>
     <row r="45" spans="1:5" s="87" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="87" t="s">
@@ -31947,7 +31926,7 @@
         <v>3626</v>
       </c>
       <c r="C86" t="s">
-        <v>3641</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -31991,10 +31970,10 @@
     </row>
     <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="166" t="s">
+      <c r="A91" s="169" t="s">
         <v>3167</v>
       </c>
-      <c r="B91" s="167"/>
+      <c r="B91" s="170"/>
     </row>
     <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="93" t="s">
@@ -32006,10 +31985,10 @@
       </c>
     </row>
     <row r="93" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="168" t="s">
+      <c r="A93" s="171" t="s">
         <v>3166</v>
       </c>
-      <c r="B93" s="169"/>
+      <c r="B93" s="172"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="86" t="s">
@@ -32021,14 +32000,14 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="165" t="s">
+      <c r="A95" s="168" t="s">
         <v>3173</v>
       </c>
-      <c r="B95" s="165"/>
+      <c r="B95" s="168"/>
     </row>
     <row r="96" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="165"/>
-      <c r="B96" s="165"/>
+      <c r="A96" s="168"/>
+      <c r="B96" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -32222,7 +32201,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>7</v>
@@ -32315,8 +32294,8 @@
         <v>No</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="160" t="s">
+    <row r="11" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="163" t="s">
         <v>3027</v>
       </c>
     </row>
@@ -32369,8 +32348,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="160" t="s">
+    <row r="17" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="163" t="s">
         <v>3028</v>
       </c>
     </row>
@@ -32418,8 +32397,8 @@
         <v>3598</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="160" t="s">
+    <row r="22" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="163" t="s">
         <v>3029</v>
       </c>
     </row>
@@ -32539,7 +32518,7 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
@@ -32557,7 +32536,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>7</v>
@@ -32580,7 +32559,7 @@
         <v>3210</v>
       </c>
       <c r="B2" t="s">
-        <v>3640</v>
+        <v>3046</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3046</v>
@@ -32648,14 +32627,14 @@
         <v>3452</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="170" t="s">
+    <row r="11" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="173" t="s">
         <v>3030</v>
       </c>
-      <c r="B11" s="171"/>
-      <c r="C11" s="171"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172"/>
+      <c r="B11" s="174"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="175"/>
     </row>
     <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
@@ -32717,7 +32696,7 @@
         <v>3400</v>
       </c>
       <c r="B17" t="s">
-        <v>3644</v>
+        <v>3639</v>
       </c>
       <c r="C17" s="139" t="s">
         <v>3619</v>
@@ -32734,14 +32713,14 @@
         <v>3562</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="170" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170" t="s">
+    <row r="19" spans="1:5" s="173" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="173" t="s">
         <v>3031</v>
       </c>
-      <c r="B19" s="171"/>
-      <c r="C19" s="171"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="171"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
     </row>
     <row r="20" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
@@ -32985,14 +32964,14 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="170" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="170" t="s">
+    <row r="42" spans="1:5" s="173" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="173" t="s">
         <v>3032</v>
       </c>
-      <c r="B42" s="171"/>
-      <c r="C42" s="171"/>
-      <c r="D42" s="171"/>
-      <c r="E42" s="171"/>
+      <c r="B42" s="174"/>
+      <c r="C42" s="174"/>
+      <c r="D42" s="174"/>
+      <c r="E42" s="174"/>
     </row>
     <row r="43" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -33010,7 +32989,7 @@
         <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>3646</v>
+        <v>3640</v>
       </c>
       <c r="C44" s="146">
         <v>14.685191</v>
@@ -33122,7 +33101,7 @@
       </c>
       <c r="B55" s="143">
         <f>SUM(B56:B57)</f>
-        <v>310000000</v>
+        <v>300000000</v>
       </c>
       <c r="C55" s="143">
         <f>SUM(C56:C57)</f>
@@ -33148,7 +33127,7 @@
       </c>
       <c r="B57" s="143">
         <f>SUMIFS('7a.Accessories'!17:17,'7a.Accessories'!12:12,B8,'7a.Accessories'!4:4,"0",'7a.Accessories'!1:1,"SUCCESS")</f>
-        <v>10000000</v>
+        <v>0</v>
       </c>
       <c r="C57" s="143">
         <f>SUMIFS('7a.Accessories'!17:17,'7a.Accessories'!12:12,C8,'7a.Accessories'!4:4,"0",'7a.Accessories'!1:1,"SUCCESS")</f>
@@ -33226,7 +33205,7 @@
       </c>
       <c r="B63" s="140">
         <f>IF(B37= "OTR-DP",B39/(B55-B61)*100,IF(B37="OTR-DP + Ins Cptlz + Fee Cptlz(Excl. Provision)",B39*100/(B55-B61+B60+(B59-B41))))</f>
-        <v>1.0163772250191419</v>
+        <v>1.0644614180045369</v>
       </c>
       <c r="C63" s="140">
         <f>IF(C37= "OTR-DP",C39/(C55-C61)*100,IF(C37="OTR-DP + Ins Cptlz + Fee Cptlz(Excl. Provision)",C39*100/(C55-C61+C60+(C59-C41))))</f>
@@ -33307,23 +33286,23 @@
       </c>
     </row>
     <row r="71" spans="1:3" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="190" t="s">
+      <c r="A71" s="157" t="s">
         <v>3485</v>
       </c>
-      <c r="B71" s="191">
+      <c r="B71" s="158">
         <v>15.651882649999999</v>
       </c>
-      <c r="C71" s="192">
+      <c r="C71" s="159">
         <v>15.67253681</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A72" s="117" t="s">
-        <v>3649</v>
+        <v>3642</v>
       </c>
       <c r="B72" s="146">
         <f>B62*100/B55</f>
-        <v>38.704838709677418</v>
+        <v>39.994999999999997</v>
       </c>
       <c r="C72" s="146">
         <f>C62*100/C55</f>
@@ -33717,10 +33696,10 @@
       <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" s="25" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183" t="s">
+      <c r="A20" s="186" t="s">
         <v>2446</v>
       </c>
-      <c r="B20" s="183"/>
+      <c r="B20" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -34082,14 +34061,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="187" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="184" t="s">
+    <row r="13" spans="1:7" s="190" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="187" t="s">
         <v>2437</v>
       </c>
-      <c r="B13" s="185"/>
-      <c r="C13" s="185"/>
-      <c r="D13" s="185"/>
-      <c r="E13" s="186"/>
+      <c r="B13" s="188"/>
+      <c r="C13" s="188"/>
+      <c r="D13" s="188"/>
+      <c r="E13" s="189"/>
     </row>
     <row r="14" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -34289,14 +34268,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="187" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="184" t="s">
+    <row r="26" spans="1:5" s="190" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="187" t="s">
         <v>2441</v>
       </c>
-      <c r="B26" s="185"/>
-      <c r="C26" s="185"/>
-      <c r="D26" s="185"/>
-      <c r="E26" s="186"/>
+      <c r="B26" s="188"/>
+      <c r="C26" s="188"/>
+      <c r="D26" s="188"/>
+      <c r="E26" s="189"/>
     </row>
     <row r="27" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -34537,11 +34516,11 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="187" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="184" t="s">
+    <row r="42" spans="1:5" s="190" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="187" t="s">
         <v>2430</v>
       </c>
-      <c r="B42" s="185"/>
+      <c r="B42" s="188"/>
     </row>
     <row r="43" spans="1:5" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
@@ -34683,8 +34662,8 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="187" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="187" t="s">
+    <row r="53" spans="1:5" s="190" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="190" t="s">
         <v>3500</v>
       </c>
     </row>
@@ -34765,10 +34744,10 @@
       <c r="B61" s="19"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="188" t="s">
+      <c r="A62" s="191" t="s">
         <v>2434</v>
       </c>
-      <c r="B62" s="189"/>
+      <c r="B62" s="192"/>
     </row>
     <row r="63" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
@@ -35061,8 +35040,8 @@
         <v>1000020</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="187" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="187" t="s">
+    <row r="18" spans="1:5" s="190" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="190" t="s">
         <v>3500</v>
       </c>
     </row>
@@ -35439,10 +35418,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -35558,10 +35537,10 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>3642</v>
+        <v>3638</v>
       </c>
       <c r="C13" t="s">
-        <v>3647</v>
+        <v>3641</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -36039,7 +36018,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:DQ492"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B43"/>
     </sheetView>
@@ -47008,10 +46987,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3645</v>
+        <v>7</v>
       </c>
       <c r="D1" s="133" t="s">
         <v>7</v>
@@ -48934,16 +48913,16 @@
       </c>
     </row>
     <row r="60" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="157" t="s">
+      <c r="A60" s="160" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="157" t="s">
+      <c r="B60" s="160" t="s">
         <v>3148</v>
       </c>
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A61" s="158"/>
-      <c r="B61" s="158"/>
+      <c r="A61" s="161"/>
+      <c r="B61" s="161"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -49143,10 +49122,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -49290,10 +49269,10 @@
       <c r="A14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="159" t="s">
+      <c r="B14" s="162" t="s">
         <v>3149</v>
       </c>
-      <c r="C14" s="159"/>
+      <c r="C14" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -49326,10 +49305,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -49458,8 +49437,8 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="160" t="s">
+    <row r="14" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="163" t="s">
         <v>3012</v>
       </c>
     </row>
@@ -49758,8 +49737,8 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="160" t="s">
+    <row r="32" spans="1:6" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="163" t="s">
         <v>3008</v>
       </c>
     </row>
@@ -49839,7 +49818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="160" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:6" s="163" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
         <v>36</v>
@@ -50199,10 +50178,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -50335,8 +50314,8 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="160" t="s">
+    <row r="14" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="163" t="s">
         <v>3012</v>
       </c>
     </row>
@@ -50468,8 +50447,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="160" t="s">
+    <row r="22" spans="1:6" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="163" t="s">
         <v>3009</v>
       </c>
     </row>
@@ -50742,10 +50721,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -50973,19 +50952,19 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>3624</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>3624</v>
@@ -51322,10 +51301,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>3637</v>
+        <v>7</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>7</v>
@@ -51345,10 +51324,10 @@
         <v>3210</v>
       </c>
       <c r="B2" t="s">
-        <v>3643</v>
+        <v>3046</v>
       </c>
       <c r="C2" t="s">
-        <v>3638</v>
+        <v>3046</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3046</v>
@@ -51413,8 +51392,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="160" t="s">
+    <row r="11" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="163" t="s">
         <v>3013</v>
       </c>
     </row>
@@ -51456,8 +51435,8 @@
         <v>3414</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="160" t="s">
+    <row r="16" spans="1:7" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="163" t="s">
         <v>3014</v>
       </c>
     </row>
@@ -51587,8 +51566,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="160" t="s">
+    <row r="29" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="163" t="s">
         <v>3015</v>
       </c>
     </row>
@@ -51738,8 +51717,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="160" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="160" t="s">
+    <row r="49" spans="1:3" s="163" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="163" t="s">
         <v>3016</v>
       </c>
     </row>
@@ -51797,8 +51776,8 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="160" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="160" t="s">
+    <row r="55" spans="1:3" s="163" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="163" t="s">
         <v>3017</v>
       </c>
     </row>
@@ -51868,8 +51847,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="160" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="160" t="s">
+    <row r="62" spans="1:3" s="163" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="163" t="s">
         <v>3490</v>
       </c>
     </row>

</xml_diff>